<commit_message>
DPE 1st wave only
</commit_message>
<xml_diff>
--- a/longitudinal/data_processing_elements_longitudinal-FRA.xlsx
+++ b/longitudinal/data_processing_elements_longitudinal-FRA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA407EF9-66D7-4A89-8186-3FBE26C21ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8A0AF2-DAF5-4AEB-95AD-2ADDB62EDA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B2BCB16-68D3-4140-81F0-4997C5056026}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="502">
   <si>
     <t>index</t>
   </si>
@@ -1880,12 +1880,6 @@
   </si>
   <si>
     <t>FRA_f1</t>
-  </si>
-  <si>
-    <t>possibly not available, need to check, not in wave2 dd but seems weird that this one was not in questionnaire</t>
-  </si>
-  <si>
-    <t>FRA_f2</t>
   </si>
 </sst>
 </file>
@@ -2274,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9590ADB0-1C2E-44B0-BD00-E7350A4F620F}">
   <dimension ref="A1:AD333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6137,7 +6131,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6193,7 +6187,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6249,7 +6243,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:24" ht="261" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="261" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6284,7 +6278,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="84" spans="1:24" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6322,3964 +6316,265 @@
         <v>500</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A85">
-        <v>1</v>
-      </c>
-      <c r="B85" t="s">
-        <v>503</v>
-      </c>
-      <c r="C85" t="s">
-        <v>30</v>
-      </c>
-      <c r="D85" t="s">
-        <v>31</v>
-      </c>
-      <c r="E85" t="s">
-        <v>32</v>
-      </c>
-      <c r="F85" t="s">
-        <v>33</v>
-      </c>
-      <c r="J85" t="s">
-        <v>34</v>
-      </c>
-      <c r="K85" t="s">
-        <v>35</v>
-      </c>
-      <c r="L85" t="s">
-        <v>36</v>
-      </c>
-      <c r="T85" t="s">
-        <v>37</v>
-      </c>
-      <c r="U85" t="s">
-        <v>38</v>
-      </c>
-      <c r="V85" t="s">
-        <v>39</v>
-      </c>
-      <c r="W85" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A86">
-        <v>2</v>
-      </c>
-      <c r="B86" t="s">
-        <v>503</v>
-      </c>
-      <c r="C86" t="s">
-        <v>40</v>
-      </c>
-      <c r="D86" t="s">
-        <v>41</v>
-      </c>
-      <c r="E86" t="s">
-        <v>41</v>
-      </c>
-      <c r="F86" t="s">
-        <v>42</v>
-      </c>
-      <c r="J86" t="s">
-        <v>43</v>
-      </c>
-      <c r="T86" t="s">
-        <v>37</v>
-      </c>
-      <c r="U86" t="s">
-        <v>38</v>
-      </c>
-      <c r="V86" t="s">
-        <v>44</v>
-      </c>
-      <c r="W86" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87">
-        <v>3</v>
-      </c>
-      <c r="B87" t="s">
-        <v>503</v>
-      </c>
-      <c r="C87" t="s">
-        <v>45</v>
-      </c>
-      <c r="D87" t="s">
-        <v>46</v>
-      </c>
-      <c r="E87" t="s">
-        <v>47</v>
-      </c>
-      <c r="F87" t="s">
-        <v>48</v>
-      </c>
-      <c r="H87" t="s">
-        <v>49</v>
-      </c>
-      <c r="J87" t="s">
-        <v>50</v>
-      </c>
-      <c r="K87" t="s">
-        <v>51</v>
-      </c>
-      <c r="L87" t="s">
-        <v>52</v>
-      </c>
-      <c r="P87" t="s">
-        <v>53</v>
-      </c>
-      <c r="T87" t="s">
-        <v>37</v>
-      </c>
-      <c r="U87" t="s">
-        <v>54</v>
-      </c>
-      <c r="V87" t="s">
-        <v>55</v>
-      </c>
-      <c r="W87" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="88" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A88">
-        <v>4</v>
-      </c>
-      <c r="B88" t="s">
-        <v>503</v>
-      </c>
-      <c r="C88" t="s">
-        <v>57</v>
-      </c>
-      <c r="D88" t="s">
-        <v>58</v>
-      </c>
-      <c r="E88" t="s">
-        <v>59</v>
-      </c>
-      <c r="F88" t="s">
-        <v>42</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J88" t="s">
-        <v>61</v>
-      </c>
-      <c r="K88" t="s">
-        <v>62</v>
-      </c>
-      <c r="L88" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q88" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="T88" t="s">
-        <v>37</v>
-      </c>
-      <c r="U88" t="s">
-        <v>38</v>
-      </c>
-      <c r="V88" t="s">
-        <v>65</v>
-      </c>
-      <c r="W88" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="89" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A89">
-        <v>5</v>
-      </c>
-      <c r="B89" t="s">
-        <v>503</v>
-      </c>
-      <c r="C89" t="s">
-        <v>67</v>
-      </c>
-      <c r="D89" t="s">
-        <v>68</v>
-      </c>
-      <c r="E89" t="s">
-        <v>69</v>
-      </c>
-      <c r="F89" t="s">
-        <v>42</v>
-      </c>
-      <c r="G89" t="s">
-        <v>70</v>
-      </c>
-      <c r="J89" t="s">
-        <v>71</v>
-      </c>
-      <c r="K89" t="s">
-        <v>72</v>
-      </c>
-      <c r="L89" t="s">
-        <v>73</v>
-      </c>
-      <c r="M89" t="s">
-        <v>74</v>
-      </c>
-      <c r="O89" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P89" t="s">
-        <v>76</v>
-      </c>
-      <c r="R89" t="s">
-        <v>70</v>
-      </c>
-      <c r="T89" t="s">
-        <v>37</v>
-      </c>
-      <c r="U89" t="s">
-        <v>38</v>
-      </c>
-      <c r="V89" t="s">
-        <v>77</v>
-      </c>
-      <c r="W89" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="90" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <v>6</v>
-      </c>
-      <c r="B90" t="s">
-        <v>503</v>
-      </c>
-      <c r="C90" t="s">
-        <v>78</v>
-      </c>
-      <c r="D90" t="s">
-        <v>79</v>
-      </c>
-      <c r="E90" t="s">
-        <v>80</v>
-      </c>
-      <c r="F90" t="s">
-        <v>42</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J90" t="s">
-        <v>43</v>
-      </c>
-      <c r="T90" t="s">
-        <v>82</v>
-      </c>
-      <c r="U90" t="s">
-        <v>83</v>
-      </c>
-      <c r="V90" t="s">
-        <v>82</v>
-      </c>
-      <c r="W90" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="91" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A91">
-        <v>7</v>
-      </c>
-      <c r="B91" t="s">
-        <v>503</v>
-      </c>
-      <c r="C91" t="s">
-        <v>84</v>
-      </c>
-      <c r="D91" t="s">
-        <v>85</v>
-      </c>
-      <c r="E91" t="s">
-        <v>86</v>
-      </c>
-      <c r="F91" t="s">
-        <v>42</v>
-      </c>
-      <c r="J91" t="s">
-        <v>87</v>
-      </c>
-      <c r="K91" t="s">
-        <v>88</v>
-      </c>
-      <c r="L91" t="s">
-        <v>89</v>
-      </c>
-      <c r="M91" t="s">
-        <v>90</v>
-      </c>
-      <c r="O91" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P91" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q91" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="T91" t="s">
-        <v>37</v>
-      </c>
-      <c r="U91" t="s">
-        <v>54</v>
-      </c>
-      <c r="V91" t="s">
-        <v>65</v>
-      </c>
-      <c r="W91" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="92" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <v>8</v>
-      </c>
-      <c r="B92" t="s">
-        <v>503</v>
-      </c>
-      <c r="C92" t="s">
-        <v>94</v>
-      </c>
-      <c r="D92" t="s">
-        <v>95</v>
-      </c>
-      <c r="E92" t="s">
-        <v>96</v>
-      </c>
-      <c r="F92" t="s">
-        <v>42</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J92" t="s">
-        <v>87</v>
-      </c>
-      <c r="K92" t="s">
-        <v>88</v>
-      </c>
-      <c r="L92" t="s">
-        <v>89</v>
-      </c>
-      <c r="M92" t="s">
-        <v>90</v>
-      </c>
-      <c r="O92" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P92" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q92" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="T92" t="s">
-        <v>37</v>
-      </c>
-      <c r="U92" t="s">
-        <v>54</v>
-      </c>
-      <c r="V92" t="s">
-        <v>65</v>
-      </c>
-      <c r="W92" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A93">
-        <v>9</v>
-      </c>
-      <c r="B93" t="s">
-        <v>503</v>
-      </c>
-      <c r="C93" t="s">
-        <v>99</v>
-      </c>
-      <c r="D93" t="s">
-        <v>100</v>
-      </c>
-      <c r="E93" t="s">
-        <v>101</v>
-      </c>
-      <c r="F93" t="s">
-        <v>102</v>
-      </c>
-      <c r="J93" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A94">
-        <v>10</v>
-      </c>
-      <c r="B94" t="s">
-        <v>503</v>
-      </c>
-      <c r="C94" t="s">
-        <v>103</v>
-      </c>
-      <c r="D94" t="s">
-        <v>104</v>
-      </c>
-      <c r="E94" t="s">
-        <v>105</v>
-      </c>
-      <c r="F94" t="s">
-        <v>33</v>
-      </c>
-      <c r="J94" t="s">
-        <v>43</v>
-      </c>
-      <c r="T94" t="s">
-        <v>82</v>
-      </c>
-      <c r="U94" t="s">
-        <v>83</v>
-      </c>
-      <c r="V94" t="s">
-        <v>82</v>
-      </c>
-      <c r="W94" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="X94" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="95" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>11</v>
-      </c>
-      <c r="B95" t="s">
-        <v>503</v>
-      </c>
-      <c r="C95" t="s">
-        <v>106</v>
-      </c>
-      <c r="D95" t="s">
-        <v>107</v>
-      </c>
-      <c r="E95" t="s">
-        <v>108</v>
-      </c>
-      <c r="F95" t="s">
-        <v>42</v>
-      </c>
-      <c r="J95" t="s">
-        <v>87</v>
-      </c>
-      <c r="K95" t="s">
-        <v>88</v>
-      </c>
-      <c r="L95" t="s">
-        <v>89</v>
-      </c>
-      <c r="M95" t="s">
-        <v>90</v>
-      </c>
-      <c r="O95" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P95" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q95" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="T95" t="s">
-        <v>37</v>
-      </c>
-      <c r="U95" t="s">
-        <v>54</v>
-      </c>
-      <c r="V95" t="s">
-        <v>65</v>
-      </c>
-      <c r="W95" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="96" spans="1:24" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>12</v>
-      </c>
-      <c r="B96" t="s">
-        <v>503</v>
-      </c>
-      <c r="C96" t="s">
-        <v>110</v>
-      </c>
-      <c r="D96" t="s">
-        <v>111</v>
-      </c>
-      <c r="E96" t="s">
-        <v>112</v>
-      </c>
-      <c r="F96" t="s">
-        <v>42</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J96" t="s">
-        <v>114</v>
-      </c>
-      <c r="K96" t="s">
-        <v>115</v>
-      </c>
-      <c r="L96" t="s">
-        <v>116</v>
-      </c>
-      <c r="M96" t="s">
-        <v>117</v>
-      </c>
-      <c r="O96" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P96" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q96" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="T96" t="s">
-        <v>37</v>
-      </c>
-      <c r="U96" t="s">
-        <v>54</v>
-      </c>
-      <c r="V96" t="s">
-        <v>65</v>
-      </c>
-      <c r="W96" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="97" spans="1:24" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>13</v>
-      </c>
-      <c r="B97" t="s">
-        <v>503</v>
-      </c>
-      <c r="C97" t="s">
-        <v>120</v>
-      </c>
-      <c r="D97" t="s">
-        <v>121</v>
-      </c>
-      <c r="E97" t="s">
-        <v>122</v>
-      </c>
-      <c r="F97" t="s">
-        <v>42</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J97" t="s">
-        <v>114</v>
-      </c>
-      <c r="K97" t="s">
-        <v>115</v>
-      </c>
-      <c r="L97" t="s">
-        <v>116</v>
-      </c>
-      <c r="M97" t="s">
-        <v>117</v>
-      </c>
-      <c r="O97" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P97" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q97" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="T97" t="s">
-        <v>37</v>
-      </c>
-      <c r="U97" t="s">
-        <v>54</v>
-      </c>
-      <c r="V97" t="s">
-        <v>65</v>
-      </c>
-      <c r="W97" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="98" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A98">
-        <v>14</v>
-      </c>
-      <c r="B98" t="s">
-        <v>503</v>
-      </c>
-      <c r="C98" t="s">
-        <v>125</v>
-      </c>
-      <c r="D98" t="s">
-        <v>126</v>
-      </c>
-      <c r="E98" t="s">
-        <v>126</v>
-      </c>
-      <c r="F98" t="s">
-        <v>42</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J98" t="s">
-        <v>43</v>
-      </c>
-      <c r="T98" t="s">
-        <v>82</v>
-      </c>
-      <c r="U98" t="s">
-        <v>83</v>
-      </c>
-      <c r="V98" t="s">
-        <v>82</v>
-      </c>
-      <c r="W98" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="99" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A99">
-        <v>15</v>
-      </c>
-      <c r="B99" t="s">
-        <v>503</v>
-      </c>
-      <c r="C99" t="s">
-        <v>128</v>
-      </c>
-      <c r="D99" t="s">
-        <v>129</v>
-      </c>
-      <c r="E99" t="s">
-        <v>129</v>
-      </c>
-      <c r="F99" t="s">
-        <v>102</v>
-      </c>
-      <c r="G99" t="s">
-        <v>130</v>
-      </c>
-      <c r="J99" t="s">
-        <v>131</v>
-      </c>
-      <c r="K99" t="s">
-        <v>132</v>
-      </c>
-      <c r="L99" t="s">
-        <v>133</v>
-      </c>
-      <c r="M99" t="s">
-        <v>134</v>
-      </c>
-      <c r="O99" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P99" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>135</v>
-      </c>
-      <c r="R99" t="s">
-        <v>130</v>
-      </c>
-      <c r="T99" t="s">
-        <v>37</v>
-      </c>
-      <c r="U99" t="s">
-        <v>38</v>
-      </c>
-      <c r="V99" t="s">
-        <v>77</v>
-      </c>
-      <c r="W99" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="100" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A100">
-        <v>16</v>
-      </c>
-      <c r="B100" t="s">
-        <v>503</v>
-      </c>
-      <c r="C100" t="s">
-        <v>136</v>
-      </c>
-      <c r="D100" t="s">
-        <v>137</v>
-      </c>
-      <c r="E100" t="s">
-        <v>137</v>
-      </c>
-      <c r="F100" t="s">
-        <v>42</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J100" t="s">
-        <v>131</v>
-      </c>
-      <c r="T100" t="s">
-        <v>37</v>
-      </c>
-      <c r="U100" t="s">
-        <v>54</v>
-      </c>
-      <c r="V100" t="s">
-        <v>55</v>
-      </c>
-      <c r="W100" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="101" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A101">
-        <v>17</v>
-      </c>
-      <c r="B101" t="s">
-        <v>503</v>
-      </c>
-      <c r="C101" t="s">
-        <v>140</v>
-      </c>
-      <c r="D101" t="s">
-        <v>141</v>
-      </c>
-      <c r="E101" t="s">
-        <v>141</v>
-      </c>
-      <c r="F101" t="s">
-        <v>102</v>
-      </c>
-      <c r="G101" t="s">
-        <v>142</v>
-      </c>
-      <c r="J101" t="s">
-        <v>143</v>
-      </c>
-      <c r="K101" t="s">
-        <v>144</v>
-      </c>
-      <c r="L101" t="s">
-        <v>145</v>
-      </c>
-      <c r="M101" t="s">
-        <v>146</v>
-      </c>
-      <c r="O101" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P101" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>135</v>
-      </c>
-      <c r="R101" t="s">
-        <v>142</v>
-      </c>
-      <c r="T101" t="s">
-        <v>37</v>
-      </c>
-      <c r="U101" t="s">
-        <v>38</v>
-      </c>
-      <c r="V101" t="s">
-        <v>77</v>
-      </c>
-      <c r="W101" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="102" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A102">
-        <v>18</v>
-      </c>
-      <c r="B102" t="s">
-        <v>503</v>
-      </c>
-      <c r="C102" t="s">
-        <v>147</v>
-      </c>
-      <c r="D102" t="s">
-        <v>148</v>
-      </c>
-      <c r="E102" t="s">
-        <v>148</v>
-      </c>
-      <c r="F102" t="s">
-        <v>42</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J102" t="s">
-        <v>143</v>
-      </c>
-      <c r="T102" t="s">
-        <v>37</v>
-      </c>
-      <c r="U102" t="s">
-        <v>54</v>
-      </c>
-      <c r="V102" t="s">
-        <v>55</v>
-      </c>
-      <c r="W102" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="103" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A103">
-        <v>19</v>
-      </c>
-      <c r="B103" t="s">
-        <v>503</v>
-      </c>
-      <c r="C103" t="s">
-        <v>150</v>
-      </c>
-      <c r="D103" t="s">
-        <v>151</v>
-      </c>
-      <c r="E103" t="s">
-        <v>151</v>
-      </c>
-      <c r="F103" t="s">
-        <v>102</v>
-      </c>
-      <c r="G103" t="s">
-        <v>152</v>
-      </c>
-      <c r="J103" t="s">
-        <v>153</v>
-      </c>
-      <c r="K103" t="s">
-        <v>154</v>
-      </c>
-      <c r="L103" t="s">
-        <v>155</v>
-      </c>
-      <c r="M103" t="s">
-        <v>156</v>
-      </c>
-      <c r="O103" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P103" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q103" t="s">
-        <v>135</v>
-      </c>
-      <c r="R103" t="s">
-        <v>152</v>
-      </c>
-      <c r="T103" t="s">
-        <v>37</v>
-      </c>
-      <c r="U103" t="s">
-        <v>38</v>
-      </c>
-      <c r="V103" t="s">
-        <v>77</v>
-      </c>
-      <c r="W103" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="104" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A104">
-        <v>20</v>
-      </c>
-      <c r="B104" t="s">
-        <v>503</v>
-      </c>
-      <c r="C104" t="s">
-        <v>157</v>
-      </c>
-      <c r="D104" t="s">
-        <v>158</v>
-      </c>
-      <c r="E104" t="s">
-        <v>158</v>
-      </c>
-      <c r="F104" t="s">
-        <v>102</v>
-      </c>
-      <c r="G104" t="s">
-        <v>130</v>
-      </c>
-      <c r="J104" t="s">
-        <v>159</v>
-      </c>
-      <c r="K104" t="s">
-        <v>160</v>
-      </c>
-      <c r="L104" t="s">
-        <v>161</v>
-      </c>
-      <c r="M104" t="s">
-        <v>162</v>
-      </c>
-      <c r="O104" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P104" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q104" t="s">
-        <v>135</v>
-      </c>
-      <c r="R104" t="s">
-        <v>163</v>
-      </c>
-      <c r="S104" t="s">
-        <v>164</v>
-      </c>
-      <c r="T104" t="s">
-        <v>37</v>
-      </c>
-      <c r="U104" t="s">
-        <v>38</v>
-      </c>
-      <c r="V104" t="s">
-        <v>77</v>
-      </c>
-      <c r="W104" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="105" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A105">
-        <v>21</v>
-      </c>
-      <c r="B105" t="s">
-        <v>503</v>
-      </c>
-      <c r="C105" t="s">
-        <v>165</v>
-      </c>
-      <c r="D105" t="s">
-        <v>166</v>
-      </c>
-      <c r="E105" t="s">
-        <v>166</v>
-      </c>
-      <c r="F105" t="s">
-        <v>42</v>
-      </c>
-      <c r="I105" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J105" t="s">
-        <v>159</v>
-      </c>
-      <c r="K105" t="s">
-        <v>160</v>
-      </c>
-      <c r="L105" t="s">
-        <v>161</v>
-      </c>
-      <c r="M105" t="s">
-        <v>162</v>
-      </c>
-      <c r="O105" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P105" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q105" t="s">
-        <v>135</v>
-      </c>
-      <c r="R105" t="s">
-        <v>163</v>
-      </c>
-      <c r="T105" t="s">
-        <v>37</v>
-      </c>
-      <c r="U105" t="s">
-        <v>54</v>
-      </c>
-      <c r="V105" t="s">
-        <v>55</v>
-      </c>
-      <c r="W105" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A106">
-        <v>22</v>
-      </c>
-      <c r="B106" t="s">
-        <v>503</v>
-      </c>
-      <c r="C106" t="s">
-        <v>168</v>
-      </c>
-      <c r="D106" t="s">
-        <v>169</v>
-      </c>
-      <c r="E106" t="s">
-        <v>169</v>
-      </c>
-      <c r="F106" t="s">
-        <v>102</v>
-      </c>
-      <c r="G106" t="s">
-        <v>170</v>
-      </c>
-      <c r="J106" t="s">
-        <v>171</v>
-      </c>
-      <c r="K106" t="s">
-        <v>172</v>
-      </c>
-      <c r="L106" t="s">
-        <v>173</v>
-      </c>
-      <c r="M106" t="s">
-        <v>174</v>
-      </c>
-      <c r="P106" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q106" t="s">
-        <v>135</v>
-      </c>
-      <c r="R106" t="s">
-        <v>170</v>
-      </c>
-      <c r="T106" t="s">
-        <v>37</v>
-      </c>
-      <c r="U106" t="s">
-        <v>38</v>
-      </c>
-      <c r="V106" t="s">
-        <v>77</v>
-      </c>
-      <c r="W106" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="X106" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="107" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A107">
-        <v>23</v>
-      </c>
-      <c r="B107" t="s">
-        <v>503</v>
-      </c>
-      <c r="C107" t="s">
-        <v>176</v>
-      </c>
-      <c r="D107" t="s">
-        <v>177</v>
-      </c>
-      <c r="E107" t="s">
-        <v>177</v>
-      </c>
-      <c r="F107" t="s">
-        <v>33</v>
-      </c>
-      <c r="J107" t="s">
-        <v>171</v>
-      </c>
-      <c r="T107" t="s">
-        <v>37</v>
-      </c>
-      <c r="U107" t="s">
-        <v>54</v>
-      </c>
-      <c r="V107" t="s">
-        <v>55</v>
-      </c>
-      <c r="W107" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="108" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A108">
-        <v>24</v>
-      </c>
-      <c r="B108" t="s">
-        <v>503</v>
-      </c>
-      <c r="C108" t="s">
-        <v>179</v>
-      </c>
-      <c r="D108" t="s">
-        <v>180</v>
-      </c>
-      <c r="E108" t="s">
-        <v>181</v>
-      </c>
-      <c r="F108" t="s">
-        <v>102</v>
-      </c>
-      <c r="G108" t="s">
-        <v>182</v>
-      </c>
-      <c r="J108" t="s">
-        <v>183</v>
-      </c>
-      <c r="K108" t="s">
-        <v>184</v>
-      </c>
-      <c r="M108" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="P108" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q108" t="s">
-        <v>135</v>
-      </c>
-      <c r="R108" t="s">
-        <v>182</v>
-      </c>
-      <c r="S108" t="s">
-        <v>186</v>
-      </c>
-      <c r="T108" t="s">
-        <v>37</v>
-      </c>
-      <c r="U108" t="s">
-        <v>54</v>
-      </c>
-      <c r="V108" t="s">
-        <v>55</v>
-      </c>
-      <c r="W108" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="109" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A109">
-        <v>25</v>
-      </c>
-      <c r="B109" t="s">
-        <v>503</v>
-      </c>
-      <c r="C109" t="s">
-        <v>188</v>
-      </c>
-      <c r="D109" t="s">
-        <v>189</v>
-      </c>
-      <c r="E109" t="s">
-        <v>190</v>
-      </c>
-      <c r="F109" t="s">
-        <v>102</v>
-      </c>
-      <c r="G109" t="s">
-        <v>182</v>
-      </c>
-      <c r="J109" t="s">
-        <v>191</v>
-      </c>
-      <c r="K109" t="s">
-        <v>192</v>
-      </c>
-      <c r="M109" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="P109" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q109" t="s">
-        <v>135</v>
-      </c>
-      <c r="R109" t="s">
-        <v>182</v>
-      </c>
-      <c r="S109" t="s">
-        <v>186</v>
-      </c>
-      <c r="T109" t="s">
-        <v>37</v>
-      </c>
-      <c r="U109" t="s">
-        <v>54</v>
-      </c>
-      <c r="V109" t="s">
-        <v>55</v>
-      </c>
-      <c r="W109" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A110">
-        <v>26</v>
-      </c>
-      <c r="B110" t="s">
-        <v>503</v>
-      </c>
-      <c r="C110" t="s">
-        <v>195</v>
-      </c>
-      <c r="D110" t="s">
-        <v>196</v>
-      </c>
-      <c r="E110" t="s">
-        <v>196</v>
-      </c>
-      <c r="F110" t="s">
-        <v>102</v>
-      </c>
-      <c r="G110" t="s">
-        <v>197</v>
-      </c>
-      <c r="J110" t="s">
-        <v>43</v>
-      </c>
-      <c r="T110" t="s">
-        <v>82</v>
-      </c>
-      <c r="U110" t="s">
-        <v>83</v>
-      </c>
-      <c r="V110" t="s">
-        <v>82</v>
-      </c>
-      <c r="W110" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A111">
-        <v>27</v>
-      </c>
-      <c r="B111" t="s">
-        <v>503</v>
-      </c>
-      <c r="C111" t="s">
-        <v>198</v>
-      </c>
-      <c r="D111" t="s">
-        <v>199</v>
-      </c>
-      <c r="E111" t="s">
-        <v>199</v>
-      </c>
-      <c r="F111" t="s">
-        <v>102</v>
-      </c>
-      <c r="G111" t="s">
-        <v>200</v>
-      </c>
-      <c r="J111" t="s">
-        <v>43</v>
-      </c>
-      <c r="T111" t="s">
-        <v>82</v>
-      </c>
-      <c r="U111" t="s">
-        <v>83</v>
-      </c>
-      <c r="V111" t="s">
-        <v>82</v>
-      </c>
-      <c r="W111" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="X111" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="112" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A112">
-        <v>28</v>
-      </c>
-      <c r="B112" t="s">
-        <v>503</v>
-      </c>
-      <c r="C112" t="s">
-        <v>202</v>
-      </c>
-      <c r="D112" t="s">
-        <v>203</v>
-      </c>
-      <c r="E112" t="s">
-        <v>203</v>
-      </c>
-      <c r="F112" t="s">
-        <v>42</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="J112" t="s">
-        <v>43</v>
-      </c>
-      <c r="T112" t="s">
-        <v>82</v>
-      </c>
-      <c r="U112" t="s">
-        <v>83</v>
-      </c>
-      <c r="V112" t="s">
-        <v>82</v>
-      </c>
-      <c r="W112" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A113">
-        <v>29</v>
-      </c>
-      <c r="B113" t="s">
-        <v>503</v>
-      </c>
-      <c r="C113" t="s">
-        <v>205</v>
-      </c>
-      <c r="D113" t="s">
-        <v>206</v>
-      </c>
-      <c r="E113" t="s">
-        <v>206</v>
-      </c>
-      <c r="F113" t="s">
-        <v>102</v>
-      </c>
-      <c r="G113" t="s">
-        <v>207</v>
-      </c>
-      <c r="J113" t="s">
-        <v>43</v>
-      </c>
-      <c r="T113" t="s">
-        <v>82</v>
-      </c>
-      <c r="U113" t="s">
-        <v>83</v>
-      </c>
-      <c r="V113" t="s">
-        <v>82</v>
-      </c>
-      <c r="W113" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A114">
-        <v>30</v>
-      </c>
-      <c r="B114" t="s">
-        <v>503</v>
-      </c>
-      <c r="C114" t="s">
-        <v>208</v>
-      </c>
-      <c r="D114" t="s">
-        <v>209</v>
-      </c>
-      <c r="E114" t="s">
-        <v>209</v>
-      </c>
-      <c r="F114" t="s">
-        <v>102</v>
-      </c>
-      <c r="G114" t="s">
-        <v>210</v>
-      </c>
-      <c r="J114" t="s">
-        <v>43</v>
-      </c>
-      <c r="T114" t="s">
-        <v>82</v>
-      </c>
-      <c r="U114" t="s">
-        <v>83</v>
-      </c>
-      <c r="V114" t="s">
-        <v>82</v>
-      </c>
-      <c r="W114" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A115">
-        <v>31</v>
-      </c>
-      <c r="B115" t="s">
-        <v>503</v>
-      </c>
-      <c r="C115" t="s">
-        <v>211</v>
-      </c>
-      <c r="D115" t="s">
-        <v>212</v>
-      </c>
-      <c r="E115" t="s">
-        <v>212</v>
-      </c>
-      <c r="F115" t="s">
-        <v>102</v>
-      </c>
-      <c r="G115" t="s">
-        <v>213</v>
-      </c>
-      <c r="J115" t="s">
-        <v>214</v>
-      </c>
-      <c r="K115" t="s">
-        <v>212</v>
-      </c>
-      <c r="L115" t="s">
-        <v>215</v>
-      </c>
-      <c r="M115" t="s">
-        <v>216</v>
-      </c>
-      <c r="T115" t="s">
-        <v>37</v>
-      </c>
-      <c r="U115" t="s">
-        <v>38</v>
-      </c>
-      <c r="V115" t="s">
-        <v>77</v>
-      </c>
-      <c r="W115" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A116">
-        <v>32</v>
-      </c>
-      <c r="B116" t="s">
-        <v>503</v>
-      </c>
-      <c r="C116" t="s">
-        <v>217</v>
-      </c>
-      <c r="D116" t="s">
-        <v>218</v>
-      </c>
-      <c r="E116" t="s">
-        <v>218</v>
-      </c>
-      <c r="F116" t="s">
-        <v>102</v>
-      </c>
-      <c r="G116" t="s">
-        <v>213</v>
-      </c>
-      <c r="J116" t="s">
-        <v>219</v>
-      </c>
-      <c r="K116" t="s">
-        <v>218</v>
-      </c>
-      <c r="L116" t="s">
-        <v>220</v>
-      </c>
-      <c r="M116" t="s">
-        <v>221</v>
-      </c>
-      <c r="T116" t="s">
-        <v>37</v>
-      </c>
-      <c r="U116" t="s">
-        <v>38</v>
-      </c>
-      <c r="V116" t="s">
-        <v>77</v>
-      </c>
-      <c r="W116" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A117">
-        <v>33</v>
-      </c>
-      <c r="B117" t="s">
-        <v>503</v>
-      </c>
-      <c r="C117" t="s">
-        <v>222</v>
-      </c>
-      <c r="D117" t="s">
-        <v>223</v>
-      </c>
-      <c r="E117" t="s">
-        <v>223</v>
-      </c>
-      <c r="F117" t="s">
-        <v>102</v>
-      </c>
-      <c r="G117" t="s">
-        <v>213</v>
-      </c>
-      <c r="J117" t="s">
-        <v>224</v>
-      </c>
-      <c r="K117" t="s">
-        <v>223</v>
-      </c>
-      <c r="L117" t="s">
-        <v>225</v>
-      </c>
-      <c r="M117" t="s">
-        <v>226</v>
-      </c>
-      <c r="T117" t="s">
-        <v>37</v>
-      </c>
-      <c r="U117" t="s">
-        <v>38</v>
-      </c>
-      <c r="V117" t="s">
-        <v>77</v>
-      </c>
-      <c r="W117" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="118" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A118">
-        <v>34</v>
-      </c>
-      <c r="B118" t="s">
-        <v>503</v>
-      </c>
-      <c r="C118" t="s">
-        <v>227</v>
-      </c>
-      <c r="D118" t="s">
-        <v>228</v>
-      </c>
-      <c r="E118" t="s">
-        <v>228</v>
-      </c>
-      <c r="F118" t="s">
-        <v>102</v>
-      </c>
-      <c r="G118" t="s">
-        <v>213</v>
-      </c>
-      <c r="J118" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K118" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="T118" t="s">
-        <v>37</v>
-      </c>
-      <c r="U118" t="s">
-        <v>54</v>
-      </c>
-      <c r="V118" t="s">
-        <v>55</v>
-      </c>
-      <c r="W118" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A119">
-        <v>35</v>
-      </c>
-      <c r="B119" t="s">
-        <v>503</v>
-      </c>
-      <c r="C119" t="s">
-        <v>232</v>
-      </c>
-      <c r="D119" t="s">
-        <v>233</v>
-      </c>
-      <c r="E119" t="s">
-        <v>233</v>
-      </c>
-      <c r="F119" t="s">
-        <v>102</v>
-      </c>
-      <c r="G119" t="s">
-        <v>213</v>
-      </c>
-      <c r="J119" t="s">
-        <v>234</v>
-      </c>
-      <c r="K119" t="s">
-        <v>233</v>
-      </c>
-      <c r="L119" t="s">
-        <v>235</v>
-      </c>
-      <c r="M119" t="s">
-        <v>236</v>
-      </c>
-      <c r="T119" t="s">
-        <v>37</v>
-      </c>
-      <c r="U119" t="s">
-        <v>38</v>
-      </c>
-      <c r="V119" t="s">
-        <v>77</v>
-      </c>
-      <c r="W119" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A120">
-        <v>36</v>
-      </c>
-      <c r="B120" t="s">
-        <v>503</v>
-      </c>
-      <c r="C120" t="s">
-        <v>237</v>
-      </c>
-      <c r="D120" t="s">
-        <v>238</v>
-      </c>
-      <c r="E120" t="s">
-        <v>238</v>
-      </c>
-      <c r="F120" t="s">
-        <v>102</v>
-      </c>
-      <c r="G120" t="s">
-        <v>239</v>
-      </c>
-      <c r="J120" t="s">
-        <v>240</v>
-      </c>
-      <c r="K120" t="s">
-        <v>238</v>
-      </c>
-      <c r="L120" t="s">
-        <v>241</v>
-      </c>
-      <c r="M120" t="s">
-        <v>242</v>
-      </c>
-      <c r="T120" t="s">
-        <v>37</v>
-      </c>
-      <c r="U120" t="s">
-        <v>38</v>
-      </c>
-      <c r="V120" t="s">
-        <v>77</v>
-      </c>
-      <c r="W120" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A121">
-        <v>37</v>
-      </c>
-      <c r="B121" t="s">
-        <v>503</v>
-      </c>
-      <c r="C121" t="s">
-        <v>243</v>
-      </c>
-      <c r="D121" t="s">
-        <v>244</v>
-      </c>
-      <c r="E121" t="s">
-        <v>245</v>
-      </c>
-      <c r="F121" t="s">
-        <v>102</v>
-      </c>
-      <c r="G121" t="s">
-        <v>246</v>
-      </c>
-      <c r="J121" t="s">
-        <v>43</v>
-      </c>
-      <c r="T121" t="s">
-        <v>82</v>
-      </c>
-      <c r="U121" t="s">
-        <v>83</v>
-      </c>
-      <c r="V121" t="s">
-        <v>82</v>
-      </c>
-      <c r="W121" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="122" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A122">
-        <v>38</v>
-      </c>
-      <c r="B122" t="s">
-        <v>503</v>
-      </c>
-      <c r="C122" t="s">
-        <v>247</v>
-      </c>
-      <c r="D122" t="s">
-        <v>248</v>
-      </c>
-      <c r="E122" t="s">
-        <v>249</v>
-      </c>
-      <c r="F122" t="s">
-        <v>42</v>
-      </c>
-      <c r="I122" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="J122" t="s">
-        <v>43</v>
-      </c>
-      <c r="T122" t="s">
-        <v>82</v>
-      </c>
-      <c r="U122" t="s">
-        <v>83</v>
-      </c>
-      <c r="V122" t="s">
-        <v>82</v>
-      </c>
-      <c r="W122" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A123">
-        <v>39</v>
-      </c>
-      <c r="B123" t="s">
-        <v>503</v>
-      </c>
-      <c r="C123" t="s">
-        <v>251</v>
-      </c>
-      <c r="D123" t="s">
-        <v>252</v>
-      </c>
-      <c r="E123" t="s">
-        <v>253</v>
-      </c>
-      <c r="F123" t="s">
-        <v>102</v>
-      </c>
-      <c r="G123" t="s">
-        <v>246</v>
-      </c>
-      <c r="J123" t="s">
-        <v>43</v>
-      </c>
-      <c r="T123" t="s">
-        <v>82</v>
-      </c>
-      <c r="U123" t="s">
-        <v>83</v>
-      </c>
-      <c r="V123" t="s">
-        <v>82</v>
-      </c>
-      <c r="W123" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="124" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A124">
-        <v>40</v>
-      </c>
-      <c r="B124" t="s">
-        <v>503</v>
-      </c>
-      <c r="C124" t="s">
-        <v>254</v>
-      </c>
-      <c r="D124" t="s">
-        <v>255</v>
-      </c>
-      <c r="E124" t="s">
-        <v>256</v>
-      </c>
-      <c r="F124" t="s">
-        <v>42</v>
-      </c>
-      <c r="I124" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="J124" t="s">
-        <v>257</v>
-      </c>
-      <c r="K124" t="s">
-        <v>258</v>
-      </c>
-      <c r="M124" t="s">
-        <v>259</v>
-      </c>
-      <c r="P124" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q124" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="T124" t="s">
-        <v>82</v>
-      </c>
-      <c r="U124" t="s">
-        <v>261</v>
-      </c>
-      <c r="V124" t="s">
-        <v>82</v>
-      </c>
-      <c r="W124" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="X124" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A125">
-        <v>41</v>
-      </c>
-      <c r="B125" t="s">
-        <v>503</v>
-      </c>
-      <c r="C125" t="s">
-        <v>263</v>
-      </c>
-      <c r="D125" t="s">
-        <v>264</v>
-      </c>
-      <c r="E125" t="s">
-        <v>264</v>
-      </c>
-      <c r="F125" t="s">
-        <v>102</v>
-      </c>
-      <c r="G125" t="s">
-        <v>265</v>
-      </c>
-      <c r="J125" t="s">
-        <v>43</v>
-      </c>
-      <c r="T125" t="s">
-        <v>82</v>
-      </c>
-      <c r="U125" t="s">
-        <v>83</v>
-      </c>
-      <c r="V125" t="s">
-        <v>82</v>
-      </c>
-      <c r="W125" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="126" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A126">
-        <v>42</v>
-      </c>
-      <c r="B126" t="s">
-        <v>503</v>
-      </c>
-      <c r="C126" t="s">
-        <v>266</v>
-      </c>
-      <c r="D126" t="s">
-        <v>267</v>
-      </c>
-      <c r="E126" t="s">
-        <v>268</v>
-      </c>
-      <c r="F126" t="s">
-        <v>102</v>
-      </c>
-      <c r="G126" t="s">
-        <v>269</v>
-      </c>
-      <c r="J126" t="s">
-        <v>270</v>
-      </c>
-      <c r="K126" t="s">
-        <v>267</v>
-      </c>
-      <c r="L126" t="s">
-        <v>271</v>
-      </c>
-      <c r="M126" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="P126" t="s">
-        <v>76</v>
-      </c>
-      <c r="T126" t="s">
-        <v>37</v>
-      </c>
-      <c r="U126" t="s">
-        <v>38</v>
-      </c>
-      <c r="V126" t="s">
-        <v>77</v>
-      </c>
-      <c r="W126" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="127" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="A127">
-        <v>43</v>
-      </c>
-      <c r="B127" t="s">
-        <v>503</v>
-      </c>
-      <c r="C127" t="s">
-        <v>273</v>
-      </c>
-      <c r="D127" t="s">
-        <v>274</v>
-      </c>
-      <c r="E127" t="s">
-        <v>274</v>
-      </c>
-      <c r="F127" t="s">
-        <v>42</v>
-      </c>
-      <c r="I127" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="J127" t="s">
-        <v>43</v>
-      </c>
-      <c r="T127" t="s">
-        <v>82</v>
-      </c>
-      <c r="U127" t="s">
-        <v>83</v>
-      </c>
-      <c r="V127" t="s">
-        <v>82</v>
-      </c>
-      <c r="W127" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="128" spans="1:24" ht="145" x14ac:dyDescent="0.35">
-      <c r="A128">
-        <v>44</v>
-      </c>
-      <c r="B128" t="s">
-        <v>503</v>
-      </c>
-      <c r="C128" t="s">
-        <v>276</v>
-      </c>
-      <c r="D128" t="s">
-        <v>277</v>
-      </c>
-      <c r="E128" t="s">
-        <v>278</v>
-      </c>
-      <c r="F128" t="s">
-        <v>42</v>
-      </c>
-      <c r="I128" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="J128" t="s">
-        <v>280</v>
-      </c>
-      <c r="K128" t="s">
-        <v>281</v>
-      </c>
-      <c r="L128" t="s">
-        <v>282</v>
-      </c>
-      <c r="M128" t="s">
-        <v>283</v>
-      </c>
-      <c r="O128" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P128" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q128" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="T128" t="s">
-        <v>37</v>
-      </c>
-      <c r="U128" t="s">
-        <v>54</v>
-      </c>
-      <c r="V128" t="s">
-        <v>65</v>
-      </c>
-      <c r="W128" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="129" spans="1:24" ht="145" x14ac:dyDescent="0.35">
-      <c r="A129">
-        <v>45</v>
-      </c>
-      <c r="B129" t="s">
-        <v>503</v>
-      </c>
-      <c r="C129" t="s">
-        <v>286</v>
-      </c>
-      <c r="D129" t="s">
-        <v>287</v>
-      </c>
-      <c r="E129" t="s">
-        <v>287</v>
-      </c>
-      <c r="F129" t="s">
-        <v>42</v>
-      </c>
-      <c r="I129" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="J129" t="s">
-        <v>43</v>
-      </c>
-      <c r="K129" t="s">
-        <v>281</v>
-      </c>
-      <c r="L129" t="s">
-        <v>282</v>
-      </c>
-      <c r="M129" t="s">
-        <v>283</v>
-      </c>
-      <c r="O129" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P129" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q129" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="T129" t="s">
-        <v>82</v>
-      </c>
-      <c r="U129" t="s">
-        <v>83</v>
-      </c>
-      <c r="V129" t="s">
-        <v>82</v>
-      </c>
-      <c r="W129" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A130">
-        <v>46</v>
-      </c>
-      <c r="B130" t="s">
-        <v>503</v>
-      </c>
-      <c r="C130" t="s">
-        <v>289</v>
-      </c>
-      <c r="D130" t="s">
-        <v>290</v>
-      </c>
-      <c r="E130" t="s">
-        <v>290</v>
-      </c>
-      <c r="F130" t="s">
-        <v>102</v>
-      </c>
-      <c r="G130" t="s">
-        <v>291</v>
-      </c>
-      <c r="J130" t="s">
-        <v>43</v>
-      </c>
-      <c r="T130" t="s">
-        <v>82</v>
-      </c>
-      <c r="U130" t="s">
-        <v>261</v>
-      </c>
-      <c r="V130" t="s">
-        <v>82</v>
-      </c>
-      <c r="W130" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="131" spans="1:24" ht="116" x14ac:dyDescent="0.35">
-      <c r="A131">
-        <v>47</v>
-      </c>
-      <c r="B131" t="s">
-        <v>503</v>
-      </c>
-      <c r="C131" t="s">
-        <v>292</v>
-      </c>
-      <c r="D131" t="s">
-        <v>293</v>
-      </c>
-      <c r="E131" t="s">
-        <v>293</v>
-      </c>
-      <c r="F131" t="s">
-        <v>42</v>
-      </c>
-      <c r="I131" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="J131" t="s">
-        <v>295</v>
-      </c>
-      <c r="K131" t="s">
-        <v>296</v>
-      </c>
-      <c r="L131" t="s">
-        <v>297</v>
-      </c>
-      <c r="M131" t="s">
-        <v>298</v>
-      </c>
-      <c r="O131" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P131" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q131" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="T131" t="s">
-        <v>37</v>
-      </c>
-      <c r="U131" t="s">
-        <v>54</v>
-      </c>
-      <c r="V131" t="s">
-        <v>65</v>
-      </c>
-      <c r="W131" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="132" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A132">
-        <v>48</v>
-      </c>
-      <c r="B132" t="s">
-        <v>503</v>
-      </c>
-      <c r="C132" t="s">
-        <v>301</v>
-      </c>
-      <c r="D132" t="s">
-        <v>302</v>
-      </c>
-      <c r="E132" t="s">
-        <v>303</v>
-      </c>
-      <c r="F132" t="s">
-        <v>42</v>
-      </c>
-      <c r="I132" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J132" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="K132" t="s">
-        <v>306</v>
-      </c>
-      <c r="L132" t="s">
-        <v>307</v>
-      </c>
-      <c r="M132" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="O132" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="P132" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q132" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="T132" t="s">
-        <v>37</v>
-      </c>
-      <c r="U132" t="s">
-        <v>54</v>
-      </c>
-      <c r="V132" t="s">
-        <v>311</v>
-      </c>
-      <c r="W132" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="133" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A133">
-        <v>49</v>
-      </c>
-      <c r="B133" t="s">
-        <v>503</v>
-      </c>
-      <c r="C133" t="s">
-        <v>313</v>
-      </c>
-      <c r="D133" t="s">
-        <v>314</v>
-      </c>
-      <c r="E133" t="s">
-        <v>315</v>
-      </c>
-      <c r="F133" t="s">
-        <v>42</v>
-      </c>
-      <c r="I133" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J133" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="K133" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="L133" t="s">
-        <v>318</v>
-      </c>
-      <c r="M133" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="O133" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="P133" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q133" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="S133" t="s">
-        <v>321</v>
-      </c>
-      <c r="T133" t="s">
-        <v>37</v>
-      </c>
-      <c r="U133" t="s">
-        <v>54</v>
-      </c>
-      <c r="V133" t="s">
-        <v>311</v>
-      </c>
-      <c r="W133" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="134" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A134">
-        <v>50</v>
-      </c>
-      <c r="B134" t="s">
-        <v>503</v>
-      </c>
-      <c r="C134" t="s">
-        <v>323</v>
-      </c>
-      <c r="D134" t="s">
-        <v>324</v>
-      </c>
-      <c r="E134" t="s">
-        <v>325</v>
-      </c>
-      <c r="F134" t="s">
-        <v>42</v>
-      </c>
-      <c r="I134" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J134" t="s">
-        <v>326</v>
-      </c>
-      <c r="K134" t="s">
-        <v>327</v>
-      </c>
-      <c r="L134" t="s">
-        <v>328</v>
-      </c>
-      <c r="M134" t="s">
-        <v>329</v>
-      </c>
-      <c r="O134" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P134" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q134" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="S134" t="s">
-        <v>331</v>
-      </c>
-      <c r="T134" t="s">
-        <v>37</v>
-      </c>
-      <c r="U134" t="s">
-        <v>54</v>
-      </c>
-      <c r="V134" t="s">
-        <v>65</v>
-      </c>
-      <c r="W134" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="135" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A135">
-        <v>51</v>
-      </c>
-      <c r="B135" t="s">
-        <v>503</v>
-      </c>
-      <c r="C135" t="s">
-        <v>332</v>
-      </c>
-      <c r="D135" t="s">
-        <v>333</v>
-      </c>
-      <c r="E135" t="s">
-        <v>334</v>
-      </c>
-      <c r="F135" t="s">
-        <v>42</v>
-      </c>
-      <c r="I135" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="J135" t="s">
-        <v>326</v>
-      </c>
-      <c r="K135" t="s">
-        <v>327</v>
-      </c>
-      <c r="L135" t="s">
-        <v>328</v>
-      </c>
-      <c r="M135" t="s">
-        <v>329</v>
-      </c>
-      <c r="O135" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P135" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q135" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="S135" t="s">
-        <v>331</v>
-      </c>
-      <c r="T135" t="s">
-        <v>37</v>
-      </c>
-      <c r="U135" t="s">
-        <v>54</v>
-      </c>
-      <c r="V135" t="s">
-        <v>65</v>
-      </c>
-      <c r="W135" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="136" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A136">
-        <v>52</v>
-      </c>
-      <c r="B136" t="s">
-        <v>503</v>
-      </c>
-      <c r="C136" t="s">
-        <v>337</v>
-      </c>
-      <c r="D136" t="s">
-        <v>338</v>
-      </c>
-      <c r="E136" t="s">
-        <v>338</v>
-      </c>
-      <c r="F136" t="s">
-        <v>42</v>
-      </c>
-      <c r="I136" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J136" t="s">
-        <v>339</v>
-      </c>
-      <c r="K136" t="s">
-        <v>340</v>
-      </c>
-      <c r="L136" t="s">
-        <v>328</v>
-      </c>
-      <c r="M136" t="s">
-        <v>341</v>
-      </c>
-      <c r="O136" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P136" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q136" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="T136" t="s">
-        <v>37</v>
-      </c>
-      <c r="U136" t="s">
-        <v>54</v>
-      </c>
-      <c r="V136" t="s">
-        <v>65</v>
-      </c>
-      <c r="W136" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="137" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A137">
-        <v>53</v>
-      </c>
-      <c r="B137" t="s">
-        <v>503</v>
-      </c>
-      <c r="C137" t="s">
-        <v>342</v>
-      </c>
-      <c r="D137" t="s">
-        <v>343</v>
-      </c>
-      <c r="E137" t="s">
-        <v>343</v>
-      </c>
-      <c r="F137" t="s">
-        <v>42</v>
-      </c>
-      <c r="I137" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J137" t="s">
-        <v>344</v>
-      </c>
-      <c r="K137" t="s">
-        <v>345</v>
-      </c>
-      <c r="L137" t="s">
-        <v>328</v>
-      </c>
-      <c r="M137" t="s">
-        <v>346</v>
-      </c>
-      <c r="O137" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P137" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q137" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="T137" t="s">
-        <v>37</v>
-      </c>
-      <c r="U137" t="s">
-        <v>54</v>
-      </c>
-      <c r="V137" t="s">
-        <v>65</v>
-      </c>
-      <c r="W137" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="138" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A138">
-        <v>54</v>
-      </c>
-      <c r="B138" t="s">
-        <v>503</v>
-      </c>
-      <c r="C138" t="s">
-        <v>348</v>
-      </c>
-      <c r="D138" t="s">
-        <v>349</v>
-      </c>
-      <c r="E138" t="s">
-        <v>349</v>
-      </c>
-      <c r="F138" t="s">
-        <v>42</v>
-      </c>
-      <c r="I138" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J138" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="K138" t="s">
-        <v>351</v>
-      </c>
-      <c r="L138" t="s">
-        <v>352</v>
-      </c>
-      <c r="M138" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="O138" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P138" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q138" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="T138" t="s">
-        <v>37</v>
-      </c>
-      <c r="U138" t="s">
-        <v>54</v>
-      </c>
-      <c r="V138" t="s">
-        <v>311</v>
-      </c>
-      <c r="W138" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="X138" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="139" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A139">
-        <v>55</v>
-      </c>
-      <c r="B139" t="s">
-        <v>503</v>
-      </c>
-      <c r="C139" t="s">
-        <v>357</v>
-      </c>
-      <c r="D139" t="s">
-        <v>358</v>
-      </c>
-      <c r="E139" t="s">
-        <v>358</v>
-      </c>
-      <c r="F139" t="s">
-        <v>42</v>
-      </c>
-      <c r="I139" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J139" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="K139" t="s">
-        <v>351</v>
-      </c>
-      <c r="L139" t="s">
-        <v>352</v>
-      </c>
-      <c r="M139" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="O139" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P139" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q139" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="T139" t="s">
-        <v>37</v>
-      </c>
-      <c r="U139" t="s">
-        <v>54</v>
-      </c>
-      <c r="V139" t="s">
-        <v>311</v>
-      </c>
-      <c r="W139" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="X139" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="140" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A140">
-        <v>56</v>
-      </c>
-      <c r="B140" t="s">
-        <v>503</v>
-      </c>
-      <c r="C140" t="s">
-        <v>360</v>
-      </c>
-      <c r="D140" t="s">
-        <v>361</v>
-      </c>
-      <c r="E140" t="s">
-        <v>361</v>
-      </c>
-      <c r="F140" t="s">
-        <v>42</v>
-      </c>
-      <c r="I140" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J140" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="K140" t="s">
-        <v>351</v>
-      </c>
-      <c r="L140" t="s">
-        <v>352</v>
-      </c>
-      <c r="M140" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="O140" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P140" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q140" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="T140" t="s">
-        <v>37</v>
-      </c>
-      <c r="U140" t="s">
-        <v>54</v>
-      </c>
-      <c r="V140" t="s">
-        <v>311</v>
-      </c>
-      <c r="W140" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="X140" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="141" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A141">
-        <v>57</v>
-      </c>
-      <c r="B141" t="s">
-        <v>503</v>
-      </c>
-      <c r="C141" t="s">
-        <v>363</v>
-      </c>
-      <c r="D141" t="s">
-        <v>364</v>
-      </c>
-      <c r="E141" t="s">
-        <v>365</v>
-      </c>
-      <c r="F141" t="s">
-        <v>42</v>
-      </c>
-      <c r="I141" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J141" t="s">
-        <v>366</v>
-      </c>
-      <c r="K141" t="s">
-        <v>367</v>
-      </c>
-      <c r="L141" t="s">
-        <v>368</v>
-      </c>
-      <c r="M141" t="s">
-        <v>369</v>
-      </c>
-      <c r="O141" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P141" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q141" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="T141" t="s">
-        <v>37</v>
-      </c>
-      <c r="U141" t="s">
-        <v>54</v>
-      </c>
-      <c r="V141" t="s">
-        <v>65</v>
-      </c>
-      <c r="W141" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A142">
-        <v>58</v>
-      </c>
-      <c r="B142" t="s">
-        <v>503</v>
-      </c>
-      <c r="C142" t="s">
-        <v>370</v>
-      </c>
-      <c r="D142" t="s">
-        <v>371</v>
-      </c>
-      <c r="E142" t="s">
-        <v>371</v>
-      </c>
-      <c r="F142" t="s">
-        <v>42</v>
-      </c>
-      <c r="J142" t="s">
-        <v>43</v>
-      </c>
-      <c r="T142" t="s">
-        <v>82</v>
-      </c>
-      <c r="U142" t="s">
-        <v>83</v>
-      </c>
-      <c r="V142" t="s">
-        <v>82</v>
-      </c>
-      <c r="W142" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A143">
-        <v>59</v>
-      </c>
-      <c r="B143" t="s">
-        <v>503</v>
-      </c>
-      <c r="C143" t="s">
-        <v>372</v>
-      </c>
-      <c r="D143" t="s">
-        <v>373</v>
-      </c>
-      <c r="E143" t="s">
-        <v>373</v>
-      </c>
-      <c r="F143" t="s">
-        <v>42</v>
-      </c>
-      <c r="J143" t="s">
-        <v>43</v>
-      </c>
-      <c r="T143" t="s">
-        <v>82</v>
-      </c>
-      <c r="U143" t="s">
-        <v>83</v>
-      </c>
-      <c r="V143" t="s">
-        <v>82</v>
-      </c>
-      <c r="W143" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A144">
-        <v>60</v>
-      </c>
-      <c r="B144" t="s">
-        <v>503</v>
-      </c>
-      <c r="C144" t="s">
-        <v>374</v>
-      </c>
-      <c r="D144" t="s">
-        <v>375</v>
-      </c>
-      <c r="E144" t="s">
-        <v>375</v>
-      </c>
-      <c r="F144" t="s">
-        <v>42</v>
-      </c>
-      <c r="J144" t="s">
-        <v>43</v>
-      </c>
-      <c r="T144" t="s">
-        <v>82</v>
-      </c>
-      <c r="U144" t="s">
-        <v>83</v>
-      </c>
-      <c r="V144" t="s">
-        <v>82</v>
-      </c>
-      <c r="W144" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A145">
-        <v>61</v>
-      </c>
-      <c r="B145" t="s">
-        <v>503</v>
-      </c>
-      <c r="C145" t="s">
-        <v>376</v>
-      </c>
-      <c r="D145" t="s">
-        <v>377</v>
-      </c>
-      <c r="E145" t="s">
-        <v>377</v>
-      </c>
-      <c r="F145" t="s">
-        <v>42</v>
-      </c>
-      <c r="J145" t="s">
-        <v>43</v>
-      </c>
-      <c r="T145" t="s">
-        <v>82</v>
-      </c>
-      <c r="U145" t="s">
-        <v>83</v>
-      </c>
-      <c r="V145" t="s">
-        <v>82</v>
-      </c>
-      <c r="W145" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A146">
-        <v>62</v>
-      </c>
-      <c r="B146" t="s">
-        <v>503</v>
-      </c>
-      <c r="C146" t="s">
-        <v>378</v>
-      </c>
-      <c r="D146" t="s">
-        <v>379</v>
-      </c>
-      <c r="E146" t="s">
-        <v>379</v>
-      </c>
-      <c r="F146" t="s">
-        <v>42</v>
-      </c>
-      <c r="J146" t="s">
-        <v>43</v>
-      </c>
-      <c r="T146" t="s">
-        <v>82</v>
-      </c>
-      <c r="U146" t="s">
-        <v>83</v>
-      </c>
-      <c r="V146" t="s">
-        <v>82</v>
-      </c>
-      <c r="W146" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="147" spans="1:23" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A147">
-        <v>63</v>
-      </c>
-      <c r="B147" t="s">
-        <v>503</v>
-      </c>
-      <c r="C147" t="s">
-        <v>380</v>
-      </c>
-      <c r="D147" t="s">
-        <v>381</v>
-      </c>
-      <c r="E147" t="s">
-        <v>381</v>
-      </c>
-      <c r="F147" t="s">
-        <v>42</v>
-      </c>
-      <c r="J147" t="s">
-        <v>382</v>
-      </c>
-      <c r="K147" t="s">
-        <v>383</v>
-      </c>
-      <c r="L147" t="s">
-        <v>384</v>
-      </c>
-      <c r="M147" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="O147" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P147" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q147" t="s">
-        <v>386</v>
-      </c>
-      <c r="T147" t="s">
-        <v>37</v>
-      </c>
-      <c r="U147" t="s">
-        <v>38</v>
-      </c>
-      <c r="V147" t="s">
-        <v>77</v>
-      </c>
-      <c r="W147" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A148">
-        <v>64</v>
-      </c>
-      <c r="B148" t="s">
-        <v>503</v>
-      </c>
-      <c r="C148" t="s">
-        <v>387</v>
-      </c>
-      <c r="D148" t="s">
-        <v>388</v>
-      </c>
-      <c r="E148" t="s">
-        <v>388</v>
-      </c>
-      <c r="F148" t="s">
-        <v>42</v>
-      </c>
-      <c r="J148" t="s">
-        <v>43</v>
-      </c>
-      <c r="T148" t="s">
-        <v>82</v>
-      </c>
-      <c r="U148" t="s">
-        <v>83</v>
-      </c>
-      <c r="V148" t="s">
-        <v>82</v>
-      </c>
-      <c r="W148" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="149" spans="1:23" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A149">
-        <v>65</v>
-      </c>
-      <c r="B149" t="s">
-        <v>503</v>
-      </c>
-      <c r="C149" t="s">
-        <v>389</v>
-      </c>
-      <c r="D149" t="s">
-        <v>390</v>
-      </c>
-      <c r="E149" t="s">
-        <v>390</v>
-      </c>
-      <c r="F149" t="s">
-        <v>42</v>
-      </c>
-      <c r="I149" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="J149" t="s">
-        <v>392</v>
-      </c>
-      <c r="K149" t="s">
-        <v>393</v>
-      </c>
-      <c r="L149" t="s">
-        <v>394</v>
-      </c>
-      <c r="M149" t="s">
-        <v>395</v>
-      </c>
-      <c r="O149" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P149" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q149" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="T149" t="s">
-        <v>37</v>
-      </c>
-      <c r="U149" t="s">
-        <v>54</v>
-      </c>
-      <c r="V149" t="s">
-        <v>65</v>
-      </c>
-      <c r="W149" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="150" spans="1:23" ht="290" x14ac:dyDescent="0.35">
-      <c r="A150">
-        <v>66</v>
-      </c>
-      <c r="B150" t="s">
-        <v>503</v>
-      </c>
-      <c r="C150" t="s">
-        <v>396</v>
-      </c>
-      <c r="D150" t="s">
-        <v>397</v>
-      </c>
-      <c r="E150" t="s">
-        <v>397</v>
-      </c>
-      <c r="F150" t="s">
-        <v>102</v>
-      </c>
-      <c r="G150" t="s">
-        <v>398</v>
-      </c>
-      <c r="J150" t="s">
-        <v>399</v>
-      </c>
-      <c r="K150" t="s">
-        <v>400</v>
-      </c>
-      <c r="L150" t="s">
-        <v>401</v>
-      </c>
-      <c r="M150" t="s">
-        <v>402</v>
-      </c>
-      <c r="O150" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="P150" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q150" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="S150" t="s">
-        <v>405</v>
-      </c>
-      <c r="T150" t="s">
-        <v>37</v>
-      </c>
-      <c r="U150" t="s">
-        <v>54</v>
-      </c>
-      <c r="V150" t="s">
-        <v>65</v>
-      </c>
-      <c r="W150" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="151" spans="1:23" ht="290" x14ac:dyDescent="0.35">
-      <c r="A151">
-        <v>67</v>
-      </c>
-      <c r="B151" t="s">
-        <v>503</v>
-      </c>
-      <c r="C151" t="s">
-        <v>407</v>
-      </c>
-      <c r="D151" t="s">
-        <v>408</v>
-      </c>
-      <c r="E151" t="s">
-        <v>408</v>
-      </c>
-      <c r="F151" t="s">
-        <v>42</v>
-      </c>
-      <c r="I151" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="J151" t="s">
-        <v>399</v>
-      </c>
-      <c r="K151" t="s">
-        <v>400</v>
-      </c>
-      <c r="L151" t="s">
-        <v>401</v>
-      </c>
-      <c r="M151" t="s">
-        <v>402</v>
-      </c>
-      <c r="O151" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="P151" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q151" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="T151" t="s">
-        <v>37</v>
-      </c>
-      <c r="U151" t="s">
-        <v>38</v>
-      </c>
-      <c r="V151" t="s">
-        <v>65</v>
-      </c>
-      <c r="W151" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="152" spans="1:23" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A152">
-        <v>68</v>
-      </c>
-      <c r="B152" t="s">
-        <v>503</v>
-      </c>
-      <c r="C152" t="s">
-        <v>411</v>
-      </c>
-      <c r="D152" t="s">
-        <v>412</v>
-      </c>
-      <c r="E152" t="s">
-        <v>412</v>
-      </c>
-      <c r="F152" t="s">
-        <v>42</v>
-      </c>
-      <c r="I152" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="J152" t="s">
-        <v>414</v>
-      </c>
-      <c r="K152" t="s">
-        <v>415</v>
-      </c>
-      <c r="L152" t="s">
-        <v>416</v>
-      </c>
-      <c r="M152" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="O152" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="P152" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q152" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="T152" t="s">
-        <v>37</v>
-      </c>
-      <c r="U152" t="s">
-        <v>54</v>
-      </c>
-      <c r="V152" t="s">
-        <v>65</v>
-      </c>
-      <c r="W152" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="153" spans="1:23" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A153">
-        <v>69</v>
-      </c>
-      <c r="B153" t="s">
-        <v>503</v>
-      </c>
-      <c r="C153" t="s">
-        <v>419</v>
-      </c>
-      <c r="D153" t="s">
-        <v>420</v>
-      </c>
-      <c r="E153" t="s">
-        <v>420</v>
-      </c>
-      <c r="F153" t="s">
-        <v>42</v>
-      </c>
-      <c r="I153" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="J153" t="s">
-        <v>422</v>
-      </c>
-      <c r="K153" t="s">
-        <v>423</v>
-      </c>
-      <c r="L153" t="s">
-        <v>424</v>
-      </c>
-      <c r="M153" t="s">
-        <v>425</v>
-      </c>
-      <c r="O153" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="P153" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q153" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="S153" t="s">
-        <v>428</v>
-      </c>
-      <c r="T153" t="s">
-        <v>37</v>
-      </c>
-      <c r="U153" t="s">
-        <v>54</v>
-      </c>
-      <c r="V153" t="s">
-        <v>65</v>
-      </c>
-      <c r="W153" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="154" spans="1:23" ht="87" x14ac:dyDescent="0.35">
-      <c r="A154">
-        <v>70</v>
-      </c>
-      <c r="B154" t="s">
-        <v>503</v>
-      </c>
-      <c r="C154" t="s">
-        <v>430</v>
-      </c>
-      <c r="D154" t="s">
-        <v>431</v>
-      </c>
-      <c r="E154" t="s">
-        <v>431</v>
-      </c>
-      <c r="F154" t="s">
-        <v>42</v>
-      </c>
-      <c r="I154" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="J154" t="s">
-        <v>43</v>
-      </c>
-      <c r="T154" t="s">
-        <v>82</v>
-      </c>
-      <c r="U154" t="s">
-        <v>83</v>
-      </c>
-      <c r="V154" t="s">
-        <v>82</v>
-      </c>
-      <c r="W154" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="155" spans="1:23" ht="87" x14ac:dyDescent="0.35">
-      <c r="A155">
-        <v>71</v>
-      </c>
-      <c r="B155" t="s">
-        <v>503</v>
-      </c>
-      <c r="C155" t="s">
-        <v>432</v>
-      </c>
-      <c r="D155" t="s">
-        <v>433</v>
-      </c>
-      <c r="E155" t="s">
-        <v>433</v>
-      </c>
-      <c r="F155" t="s">
-        <v>42</v>
-      </c>
-      <c r="I155" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="J155" t="s">
-        <v>43</v>
-      </c>
-      <c r="T155" t="s">
-        <v>82</v>
-      </c>
-      <c r="U155" t="s">
-        <v>83</v>
-      </c>
-      <c r="V155" t="s">
-        <v>82</v>
-      </c>
-      <c r="W155" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="156" spans="1:23" ht="319" x14ac:dyDescent="0.35">
-      <c r="A156">
-        <v>72</v>
-      </c>
-      <c r="B156" t="s">
-        <v>503</v>
-      </c>
-      <c r="C156" t="s">
-        <v>434</v>
-      </c>
-      <c r="D156" t="s">
-        <v>435</v>
-      </c>
-      <c r="E156" t="s">
-        <v>436</v>
-      </c>
-      <c r="F156" t="s">
-        <v>42</v>
-      </c>
-      <c r="I156" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="J156" t="s">
-        <v>438</v>
-      </c>
-      <c r="K156" t="s">
-        <v>439</v>
-      </c>
-      <c r="L156" t="s">
-        <v>440</v>
-      </c>
-      <c r="M156" t="s">
-        <v>441</v>
-      </c>
-      <c r="O156" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="P156" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q156" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="S156" t="s">
-        <v>442</v>
-      </c>
-      <c r="T156" t="s">
-        <v>37</v>
-      </c>
-      <c r="U156" t="s">
-        <v>38</v>
-      </c>
-      <c r="V156" t="s">
-        <v>55</v>
-      </c>
-      <c r="W156" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="157" spans="1:23" ht="87" x14ac:dyDescent="0.35">
-      <c r="A157">
-        <v>73</v>
-      </c>
-      <c r="B157" t="s">
-        <v>503</v>
-      </c>
-      <c r="C157" t="s">
-        <v>444</v>
-      </c>
-      <c r="D157" t="s">
-        <v>445</v>
-      </c>
-      <c r="E157" t="s">
-        <v>446</v>
-      </c>
-      <c r="F157" t="s">
-        <v>42</v>
-      </c>
-      <c r="I157" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="J157" t="s">
-        <v>43</v>
-      </c>
-      <c r="T157" t="s">
-        <v>82</v>
-      </c>
-      <c r="U157" t="s">
-        <v>83</v>
-      </c>
-      <c r="V157" t="s">
-        <v>82</v>
-      </c>
-      <c r="W157" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="158" spans="1:23" ht="87" x14ac:dyDescent="0.35">
-      <c r="A158">
-        <v>74</v>
-      </c>
-      <c r="B158" t="s">
-        <v>503</v>
-      </c>
-      <c r="C158" t="s">
-        <v>447</v>
-      </c>
-      <c r="D158" t="s">
-        <v>448</v>
-      </c>
-      <c r="E158" t="s">
-        <v>449</v>
-      </c>
-      <c r="F158" t="s">
-        <v>42</v>
-      </c>
-      <c r="I158" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="J158" t="s">
-        <v>43</v>
-      </c>
-      <c r="T158" t="s">
-        <v>82</v>
-      </c>
-      <c r="U158" t="s">
-        <v>83</v>
-      </c>
-      <c r="V158" t="s">
-        <v>82</v>
-      </c>
-      <c r="W158" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="159" spans="1:23" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A159">
-        <v>75</v>
-      </c>
-      <c r="B159" t="s">
-        <v>503</v>
-      </c>
-      <c r="C159" t="s">
-        <v>450</v>
-      </c>
-      <c r="D159" t="s">
-        <v>451</v>
-      </c>
-      <c r="E159" t="s">
-        <v>452</v>
-      </c>
-      <c r="F159" t="s">
-        <v>42</v>
-      </c>
-      <c r="G159" t="s">
-        <v>398</v>
-      </c>
-      <c r="J159" t="s">
-        <v>453</v>
-      </c>
-      <c r="K159" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="L159" t="s">
-        <v>455</v>
-      </c>
-      <c r="M159" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="O159" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="P159" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q159" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="S159" t="s">
-        <v>457</v>
-      </c>
-      <c r="T159" t="s">
-        <v>37</v>
-      </c>
-      <c r="U159" t="s">
-        <v>54</v>
-      </c>
-      <c r="V159" t="s">
-        <v>55</v>
-      </c>
-      <c r="W159" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="160" spans="1:23" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A160">
-        <v>76</v>
-      </c>
-      <c r="B160" t="s">
-        <v>503</v>
-      </c>
-      <c r="C160" t="s">
-        <v>459</v>
-      </c>
-      <c r="D160" t="s">
-        <v>460</v>
-      </c>
-      <c r="E160" t="s">
-        <v>461</v>
-      </c>
-      <c r="F160" t="s">
-        <v>42</v>
-      </c>
-      <c r="I160" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="J160" t="s">
-        <v>453</v>
-      </c>
-      <c r="K160" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="L160" t="s">
-        <v>455</v>
-      </c>
-      <c r="M160" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="O160" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="P160" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q160" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="S160" t="s">
-        <v>457</v>
-      </c>
-      <c r="T160" t="s">
-        <v>37</v>
-      </c>
-      <c r="U160" t="s">
-        <v>54</v>
-      </c>
-      <c r="V160" t="s">
-        <v>311</v>
-      </c>
-      <c r="W160" s="1" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="161" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A161">
-        <v>77</v>
-      </c>
-      <c r="B161" t="s">
-        <v>503</v>
-      </c>
-      <c r="C161" t="s">
-        <v>464</v>
-      </c>
-      <c r="D161" t="s">
-        <v>465</v>
-      </c>
-      <c r="E161" t="s">
-        <v>466</v>
-      </c>
-      <c r="F161" t="s">
-        <v>42</v>
-      </c>
-      <c r="I161" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="J161" t="s">
-        <v>43</v>
-      </c>
-      <c r="T161" t="s">
-        <v>82</v>
-      </c>
-      <c r="U161" t="s">
-        <v>261</v>
-      </c>
-      <c r="V161" t="s">
-        <v>82</v>
-      </c>
-      <c r="W161" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="162" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A162">
-        <v>78</v>
-      </c>
-      <c r="B162" t="s">
-        <v>503</v>
-      </c>
-      <c r="C162" t="s">
-        <v>468</v>
-      </c>
-      <c r="D162" t="s">
-        <v>469</v>
-      </c>
-      <c r="E162" t="s">
-        <v>469</v>
-      </c>
-      <c r="F162" t="s">
-        <v>42</v>
-      </c>
-      <c r="I162" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="J162" t="s">
-        <v>43</v>
-      </c>
-      <c r="T162" t="s">
-        <v>82</v>
-      </c>
-      <c r="U162" t="s">
-        <v>261</v>
-      </c>
-      <c r="V162" t="s">
-        <v>82</v>
-      </c>
-      <c r="W162" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="163" spans="1:24" ht="29" x14ac:dyDescent="0.35">
-      <c r="A163">
-        <v>79</v>
-      </c>
-      <c r="B163" t="s">
-        <v>503</v>
-      </c>
-      <c r="C163" t="s">
-        <v>471</v>
-      </c>
-      <c r="D163" t="s">
-        <v>472</v>
-      </c>
-      <c r="E163" t="s">
-        <v>473</v>
-      </c>
-      <c r="F163" t="s">
-        <v>42</v>
-      </c>
-      <c r="I163" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J163" t="s">
-        <v>43</v>
-      </c>
-      <c r="T163" t="s">
-        <v>82</v>
-      </c>
-      <c r="U163" t="s">
-        <v>83</v>
-      </c>
-      <c r="V163" t="s">
-        <v>82</v>
-      </c>
-      <c r="W163" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="164" spans="1:24" ht="290" x14ac:dyDescent="0.35">
-      <c r="A164">
-        <v>80</v>
-      </c>
-      <c r="B164" t="s">
-        <v>503</v>
-      </c>
-      <c r="C164" t="s">
-        <v>474</v>
-      </c>
-      <c r="D164" t="s">
-        <v>475</v>
-      </c>
-      <c r="E164" t="s">
-        <v>476</v>
-      </c>
-      <c r="F164" t="s">
-        <v>42</v>
-      </c>
-      <c r="I164" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J164" t="s">
-        <v>477</v>
-      </c>
-      <c r="K164" t="s">
-        <v>478</v>
-      </c>
-      <c r="L164" t="s">
-        <v>479</v>
-      </c>
-      <c r="M164" t="s">
-        <v>480</v>
-      </c>
-      <c r="O164" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P164" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q164" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="T164" t="s">
-        <v>37</v>
-      </c>
-      <c r="U164" t="s">
-        <v>54</v>
-      </c>
-      <c r="V164" t="s">
-        <v>65</v>
-      </c>
-      <c r="W164" s="1" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="165" spans="1:24" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A165">
-        <v>81</v>
-      </c>
-      <c r="B165" t="s">
-        <v>503</v>
-      </c>
-      <c r="C165" t="s">
-        <v>483</v>
-      </c>
-      <c r="D165" t="s">
-        <v>484</v>
-      </c>
-      <c r="E165" t="s">
-        <v>485</v>
-      </c>
-      <c r="F165" t="s">
-        <v>42</v>
-      </c>
-      <c r="I165" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="J165" t="s">
-        <v>486</v>
-      </c>
-      <c r="K165" t="s">
-        <v>487</v>
-      </c>
-      <c r="L165" t="s">
-        <v>488</v>
-      </c>
-      <c r="M165" t="s">
-        <v>489</v>
-      </c>
-      <c r="O165" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P165" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q165" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="T165" t="s">
-        <v>82</v>
-      </c>
-      <c r="U165" t="s">
-        <v>83</v>
-      </c>
-      <c r="V165" t="s">
-        <v>82</v>
-      </c>
-      <c r="W165" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="X165" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="166" spans="1:24" ht="261" x14ac:dyDescent="0.35">
-      <c r="A166">
-        <v>82</v>
-      </c>
-      <c r="B166" t="s">
-        <v>503</v>
-      </c>
-      <c r="C166" t="s">
-        <v>491</v>
-      </c>
-      <c r="D166" t="s">
-        <v>492</v>
-      </c>
-      <c r="E166" t="s">
-        <v>493</v>
-      </c>
-      <c r="F166" t="s">
-        <v>102</v>
-      </c>
-      <c r="J166" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="T166" t="s">
-        <v>37</v>
-      </c>
-      <c r="U166" t="s">
-        <v>54</v>
-      </c>
-      <c r="V166" t="s">
-        <v>55</v>
-      </c>
-      <c r="W166" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="167" spans="1:24" ht="362.5" x14ac:dyDescent="0.35">
-      <c r="A167">
-        <v>83</v>
-      </c>
-      <c r="B167" t="s">
-        <v>503</v>
-      </c>
-      <c r="C167" t="s">
-        <v>496</v>
-      </c>
-      <c r="D167" t="s">
-        <v>497</v>
-      </c>
-      <c r="E167" t="s">
-        <v>498</v>
-      </c>
-      <c r="F167" t="s">
-        <v>42</v>
-      </c>
-      <c r="G167" t="s">
-        <v>499</v>
-      </c>
-      <c r="J167" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="T167" t="s">
-        <v>37</v>
-      </c>
-      <c r="U167" t="s">
-        <v>54</v>
-      </c>
-      <c r="V167" t="s">
-        <v>55</v>
-      </c>
-      <c r="W167" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I88" s="1"/>
+      <c r="Q88" s="1"/>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="O89" s="1"/>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="O91" s="1"/>
+      <c r="Q91" s="1"/>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="Q92" s="1"/>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="O95" s="1"/>
+      <c r="Q95" s="1"/>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="Q96" s="1"/>
+    </row>
+    <row r="97" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="Q97" s="1"/>
+    </row>
+    <row r="98" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="O99" s="1"/>
+    </row>
+    <row r="100" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="O101" s="1"/>
+    </row>
+    <row r="102" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="O103" s="1"/>
+    </row>
+    <row r="104" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="O104" s="1"/>
+    </row>
+    <row r="105" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I105" s="1"/>
+      <c r="O105" s="1"/>
+    </row>
+    <row r="108" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="M108" s="1"/>
+    </row>
+    <row r="109" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="M109" s="1"/>
+    </row>
+    <row r="112" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I112" s="1"/>
+    </row>
+    <row r="118" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+    </row>
+    <row r="122" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I122" s="1"/>
+    </row>
+    <row r="124" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I124" s="1"/>
+      <c r="Q124" s="1"/>
+    </row>
+    <row r="126" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="M126" s="1"/>
+    </row>
+    <row r="127" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I128" s="1"/>
+      <c r="O128" s="1"/>
+      <c r="Q128" s="1"/>
+    </row>
+    <row r="129" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I129" s="1"/>
+      <c r="O129" s="1"/>
+      <c r="Q129" s="1"/>
+    </row>
+    <row r="131" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I131" s="1"/>
+      <c r="O131" s="1"/>
+      <c r="Q131" s="1"/>
+    </row>
+    <row r="132" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="O132" s="1"/>
+      <c r="Q132" s="1"/>
+    </row>
+    <row r="133" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="O133" s="1"/>
+      <c r="Q133" s="1"/>
+    </row>
+    <row r="134" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I134" s="1"/>
+      <c r="O134" s="1"/>
+      <c r="Q134" s="1"/>
+    </row>
+    <row r="135" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I135" s="1"/>
+      <c r="O135" s="1"/>
+      <c r="Q135" s="1"/>
+    </row>
+    <row r="136" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I136" s="1"/>
+      <c r="O136" s="1"/>
+      <c r="Q136" s="1"/>
+    </row>
+    <row r="137" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I137" s="1"/>
+      <c r="O137" s="1"/>
+      <c r="Q137" s="1"/>
+    </row>
+    <row r="138" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="M138" s="1"/>
+      <c r="O138" s="1"/>
+      <c r="Q138" s="1"/>
+    </row>
+    <row r="139" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="M139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="Q139" s="1"/>
+    </row>
+    <row r="140" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="M140" s="1"/>
+      <c r="O140" s="1"/>
+      <c r="Q140" s="1"/>
+    </row>
+    <row r="141" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I141" s="1"/>
+      <c r="O141" s="1"/>
+      <c r="Q141" s="1"/>
+    </row>
+    <row r="147" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="M147" s="1"/>
+      <c r="O147" s="1"/>
+    </row>
+    <row r="149" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I149" s="1"/>
+      <c r="O149" s="1"/>
+      <c r="Q149" s="1"/>
+    </row>
+    <row r="150" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="O150" s="1"/>
+      <c r="Q150" s="1"/>
+    </row>
+    <row r="151" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="Q151" s="1"/>
+    </row>
+    <row r="152" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I152" s="1"/>
+      <c r="M152" s="1"/>
+      <c r="O152" s="1"/>
+      <c r="Q152" s="1"/>
+    </row>
+    <row r="153" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I153" s="1"/>
+      <c r="O153" s="1"/>
+      <c r="Q153" s="1"/>
+    </row>
+    <row r="154" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I154" s="1"/>
+    </row>
+    <row r="155" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I155" s="1"/>
+    </row>
+    <row r="156" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I156" s="1"/>
+      <c r="O156" s="1"/>
+      <c r="Q156" s="1"/>
+    </row>
+    <row r="157" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I157" s="1"/>
+    </row>
+    <row r="158" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I158" s="1"/>
+    </row>
+    <row r="159" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="K159" s="1"/>
+      <c r="M159" s="1"/>
+      <c r="O159" s="1"/>
+      <c r="Q159" s="1"/>
+    </row>
+    <row r="160" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="O160" s="1"/>
+      <c r="Q160" s="1"/>
+    </row>
+    <row r="161" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I161" s="1"/>
+    </row>
+    <row r="162" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I162" s="1"/>
+    </row>
+    <row r="163" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I163" s="1"/>
+    </row>
+    <row r="164" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I164" s="1"/>
+      <c r="O164" s="1"/>
+      <c r="Q164" s="1"/>
+    </row>
+    <row r="165" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I165" s="1"/>
+      <c r="O165" s="1"/>
+      <c r="Q165" s="1"/>
+    </row>
+    <row r="166" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="J166" s="1"/>
+    </row>
+    <row r="167" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="J167" s="1"/>
+    </row>
+    <row r="171" spans="9:17" x14ac:dyDescent="0.35">
       <c r="I171" s="1"/>
       <c r="Q171" s="1"/>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="172" spans="9:17" x14ac:dyDescent="0.35">
       <c r="O172" s="1"/>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="173" spans="9:17" x14ac:dyDescent="0.35">
       <c r="I173" s="1"/>
     </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="174" spans="9:17" x14ac:dyDescent="0.35">
       <c r="O174" s="1"/>
       <c r="Q174" s="1"/>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="175" spans="9:17" x14ac:dyDescent="0.35">
       <c r="I175" s="1"/>
       <c r="O175" s="1"/>
       <c r="Q175" s="1"/>

</xml_diff>

<commit_message>
1st follow-up wave only
</commit_message>
<xml_diff>
--- a/longitudinal/data_processing_elements_longitudinal-FRA.xlsx
+++ b/longitudinal/data_processing_elements_longitudinal-FRA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8A0AF2-DAF5-4AEB-95AD-2ADDB62EDA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A9A0F9-7007-478A-87E5-2757FD8B202A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B2BCB16-68D3-4140-81F0-4997C5056026}"/>
   </bookViews>
@@ -2268,12 +2268,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9590ADB0-1C2E-44B0-BD00-E7350A4F620F}">
   <dimension ref="A1:AD333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
     <col min="3" max="3" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.26953125" customWidth="1"/>
     <col min="5" max="5" width="24.54296875" customWidth="1"/>

</xml_diff>

<commit_message>
correct variable names and undetermined
</commit_message>
<xml_diff>
--- a/longitudinal/data_processing_elements_longitudinal-FRA.xlsx
+++ b/longitudinal/data_processing_elements_longitudinal-FRA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25FFD0B-1CC9-4BBF-B0D8-D9BDC6E0A6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378BB681-8F85-494B-AD37-571558CD8070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4B2BCB16-68D3-4140-81F0-4997C5056026}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3548" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3552" uniqueCount="619">
   <si>
     <t>index</t>
   </si>
@@ -1723,50 +1723,6 @@
 med9atc_w2</t>
   </si>
   <si>
-    <t>case_when(
-med1atc_w2 == "X04" ~ 1L;
-med2atc_w2 == "X04" ~ 1L;
-med3atc_w2 == "X04" ~ 1L;
-med4atc_w2 == "X04" ~ 1L;
-med5atc_w2 == "X04" ~ 1L;
-med6atc_w2 == "X04" ~ 1L;
-med7atc_w2 == "X04" ~ 1L;
-med8atc_w2 == "X04" ~ 1L;
-med9atc_w2 == "X04" ~ 1L;
-grepl("^C10", med1atc_w2, ignore.case = TRUE) ~ 1L;
-grepl("^C10", med2atc_w2, ignore.case = TRUE) ~ 1L;
-grepl("^C10", med3atc_w2, ignore.case = TRUE) ~ 1L;
-grepl("^C10", med4atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C10", med5atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C10", med6atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C10", med7atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C10", med8atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C10", med9atc1, ignore.case = TRUE) ~ 1L;
-ELSE ~ 0L)</t>
-  </si>
-  <si>
-    <t>case_when(
-med1atc_w2 == "X01" ~ 1L;
-med2atc_w2 == "X01" ~ 1L;
-med3atc_w2 == "X01" ~ 1L;
-med4atc_w2 == "X01" ~ 1L;
-med5atc_w2 == "X01" ~ 1L;
-med6atc_w2 == "X01" ~ 1L;
-med7atc_w2== "X01" ~ 1L;
-med8atc_w2 == "X01" ~ 1L;
-med9atc_w2 == "X01" ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med1atc_w2, ignore.case = TRUE) ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med2atc_w2, ignore.case = TRUE) ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med3atc_w2, ignore.case = TRUE) ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med4atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med5atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med6atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med7atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med8atc1, ignore.case = TRUE) ~ 1L;
-grepl("^C02|^C03|^C07|^C08|^C09", med9atc1, ignore.case = TRUE) ~ 1L;
-ELSE ~ 0L)</t>
-  </si>
-  <si>
     <t>depression_w2</t>
   </si>
   <si>
@@ -2325,15 +2281,6 @@
 mutate(phy_SF36_nb_items = if_else(phy_SF36_nb_items == 0, NA, phy_SF36_nb_items)</t>
   </si>
   <si>
-    <t>highcholesterol</t>
-  </si>
-  <si>
-    <t>malignanttumor</t>
-  </si>
-  <si>
-    <t>diabetes</t>
-  </si>
-  <si>
     <t>smoking_status_w2</t>
   </si>
   <si>
@@ -2365,9 +2312,6 @@
 ELSE ~ 0L)</t>
   </si>
   <si>
-    <t>bmi</t>
-  </si>
-  <si>
     <t>waist_mean_w3</t>
   </si>
   <si>
@@ -2476,10 +2420,66 @@
 mutate(phy_SF36_nb_items = if_else(phy_SF36_nb_items == 0, NA, phy_SF36_nb_items)</t>
   </si>
   <si>
-    <t>mci</t>
-  </si>
-  <si>
     <t>smoking_status_w3</t>
+  </si>
+  <si>
+    <t>diabetes_w2</t>
+  </si>
+  <si>
+    <t>malignanttumor_w2</t>
+  </si>
+  <si>
+    <t>highcholesterol_w2</t>
+  </si>
+  <si>
+    <t>case_when(
+med1atc_w2 == "X04" ~ 1L;
+med2atc_w2 == "X04" ~ 1L;
+med3atc_w2 == "X04" ~ 1L;
+med4atc_w2 == "X04" ~ 1L;
+med5atc_w2 == "X04" ~ 1L;
+med6atc_w2 == "X04" ~ 1L;
+med7atc_w2 == "X04" ~ 1L;
+med8atc_w2 == "X04" ~ 1L;
+med9atc_w2 == "X04" ~ 1L;
+grepl("^C10", med1atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C10", med2atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C10", med3atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C10", med4atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C10", med5atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C10", med6atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C10", med7atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C10", med8atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C10", med9atc_w2, ignore.case = TRUE) ~ 1L;
+ELSE ~ 0L)</t>
+  </si>
+  <si>
+    <t>case_when(
+med1atc_w2 == "X01" ~ 1L;
+med2atc_w2 == "X01" ~ 1L;
+med3atc_w2 == "X01" ~ 1L;
+med4atc_w2 == "X01" ~ 1L;
+med5atc_w2 == "X01" ~ 1L;
+med6atc_w2 == "X01" ~ 1L;
+med7atc_w2== "X01" ~ 1L;
+med8atc_w2 == "X01" ~ 1L;
+med9atc_w2 == "X01" ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med1atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med2atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med3atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med4atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med5atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med6atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med7atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med8atc_w2, ignore.case = TRUE) ~ 1L;
+grepl("^C02|^C03|^C07|^C08|^C09", med9atc_w2, ignore.case = TRUE) ~ 1L;
+ELSE ~ 0L)</t>
+  </si>
+  <si>
+    <t>bmi_w3</t>
+  </si>
+  <si>
+    <t>mci_w3</t>
   </si>
 </sst>
 </file>
@@ -2874,8 +2874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9590ADB0-1C2E-44B0-BD00-E7350A4F620F}">
   <dimension ref="A1:AD333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J126" sqref="J126"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R174" sqref="R174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3913,7 +3913,7 @@
         <v>125</v>
       </c>
       <c r="J21" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="K21" t="s">
         <v>149</v>
@@ -3975,7 +3975,7 @@
         <v>132</v>
       </c>
       <c r="J22" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="K22" t="s">
         <v>149</v>
@@ -4008,7 +4008,7 @@
         <v>54</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4999,7 +4999,7 @@
         <v>252</v>
       </c>
       <c r="J45" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="K45" t="s">
         <v>253</v>
@@ -5320,7 +5320,7 @@
         <v>275</v>
       </c>
       <c r="J51" t="s">
-        <v>599</v>
+        <v>612</v>
       </c>
       <c r="K51" t="s">
         <v>293</v>
@@ -5379,7 +5379,7 @@
         <v>301</v>
       </c>
       <c r="J52" t="s">
-        <v>599</v>
+        <v>612</v>
       </c>
       <c r="K52" t="s">
         <v>293</v>
@@ -5438,7 +5438,7 @@
         <v>275</v>
       </c>
       <c r="J53" t="s">
-        <v>598</v>
+        <v>613</v>
       </c>
       <c r="K53" t="s">
         <v>305</v>
@@ -5494,7 +5494,7 @@
         <v>275</v>
       </c>
       <c r="J54" t="s">
-        <v>597</v>
+        <v>614</v>
       </c>
       <c r="K54" t="s">
         <v>309</v>
@@ -5580,7 +5580,7 @@
         <v>281</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>482</v>
+        <v>615</v>
       </c>
       <c r="X55" t="s">
         <v>318</v>
@@ -5639,7 +5639,7 @@
         <v>281</v>
       </c>
       <c r="W56" s="1" t="s">
-        <v>483</v>
+        <v>616</v>
       </c>
       <c r="X56" t="s">
         <v>318</v>
@@ -5698,7 +5698,7 @@
         <v>281</v>
       </c>
       <c r="W57" s="1" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="X57" t="s">
         <v>318</v>
@@ -5727,7 +5727,7 @@
         <v>275</v>
       </c>
       <c r="J58" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K58" t="s">
         <v>326</v>
@@ -5955,7 +5955,7 @@
         <v>42</v>
       </c>
       <c r="J64" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="K64" t="s">
         <v>341</v>
@@ -6046,7 +6046,7 @@
         <v>349</v>
       </c>
       <c r="J66" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="K66" t="s">
         <v>350</v>
@@ -6102,7 +6102,7 @@
         <v>355</v>
       </c>
       <c r="J67" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="K67" t="s">
         <v>356</v>
@@ -6161,7 +6161,7 @@
         <v>365</v>
       </c>
       <c r="J68" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="K68" t="s">
         <v>356</v>
@@ -6217,7 +6217,7 @@
         <v>369</v>
       </c>
       <c r="J69" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="K69" t="s">
         <v>370</v>
@@ -6273,7 +6273,7 @@
         <v>376</v>
       </c>
       <c r="J70" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="K70" t="s">
         <v>377</v>
@@ -6408,7 +6408,7 @@
         <v>391</v>
       </c>
       <c r="J73" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K73" t="s">
         <v>392</v>
@@ -6441,7 +6441,7 @@
         <v>54</v>
       </c>
       <c r="W73" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="74" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -6543,7 +6543,7 @@
         <v>355</v>
       </c>
       <c r="J76" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>405</v>
@@ -6573,7 +6573,7 @@
         <v>54</v>
       </c>
       <c r="W76" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="77" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
@@ -6599,7 +6599,7 @@
         <v>412</v>
       </c>
       <c r="J77" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>405</v>
@@ -6629,7 +6629,7 @@
         <v>281</v>
       </c>
       <c r="W77" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="78" spans="1:23" ht="75" x14ac:dyDescent="0.25">
@@ -6769,7 +6769,7 @@
         <v>275</v>
       </c>
       <c r="J81" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="K81" t="s">
         <v>426</v>
@@ -6825,7 +6825,7 @@
         <v>275</v>
       </c>
       <c r="J82" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="K82" t="s">
         <v>434</v>
@@ -6878,7 +6878,7 @@
         <v>98</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="T83" t="s">
         <v>37</v>
@@ -6890,7 +6890,7 @@
         <v>54</v>
       </c>
       <c r="W83" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="84" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -6916,7 +6916,7 @@
         <v>444</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="T84" t="s">
         <v>37</v>
@@ -6928,7 +6928,7 @@
         <v>54</v>
       </c>
       <c r="W84" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
@@ -7030,7 +7030,7 @@
         <v>49</v>
       </c>
       <c r="J87" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="K87" t="s">
         <v>50</v>
@@ -7051,7 +7051,7 @@
         <v>54</v>
       </c>
       <c r="W87" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="88" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7124,7 +7124,7 @@
         <v>68</v>
       </c>
       <c r="J89" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K89" t="s">
         <v>69</v>
@@ -7215,7 +7215,7 @@
         <v>42</v>
       </c>
       <c r="J91" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="K91" t="s">
         <v>84</v>
@@ -7271,7 +7271,7 @@
         <v>93</v>
       </c>
       <c r="J92" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="K92" t="s">
         <v>84</v>
@@ -7397,7 +7397,7 @@
         <v>42</v>
       </c>
       <c r="J95" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="K95" t="s">
         <v>84</v>
@@ -7453,7 +7453,7 @@
         <v>109</v>
       </c>
       <c r="J96" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K96" t="s">
         <v>110</v>
@@ -7509,7 +7509,7 @@
         <v>118</v>
       </c>
       <c r="J97" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K97" t="s">
         <v>110</v>
@@ -7603,7 +7603,7 @@
         <v>125</v>
       </c>
       <c r="J99" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K99" t="s">
         <v>126</v>
@@ -7662,7 +7662,7 @@
         <v>132</v>
       </c>
       <c r="J100" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="T100" t="s">
         <v>37</v>
@@ -7674,7 +7674,7 @@
         <v>54</v>
       </c>
       <c r="W100" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="101" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -7700,7 +7700,7 @@
         <v>135</v>
       </c>
       <c r="J101" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="K101" t="s">
         <v>136</v>
@@ -7759,7 +7759,7 @@
         <v>132</v>
       </c>
       <c r="J102" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="T102" t="s">
         <v>37</v>
@@ -7771,7 +7771,7 @@
         <v>54</v>
       </c>
       <c r="W102" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="103" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -7797,7 +7797,7 @@
         <v>143</v>
       </c>
       <c r="J103" t="s">
-        <v>604</v>
+        <v>617</v>
       </c>
       <c r="K103" t="s">
         <v>144</v>
@@ -7856,7 +7856,7 @@
         <v>125</v>
       </c>
       <c r="J104" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="K104" t="s">
         <v>149</v>
@@ -7918,7 +7918,7 @@
         <v>132</v>
       </c>
       <c r="J105" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="K105" t="s">
         <v>149</v>
@@ -7951,7 +7951,7 @@
         <v>54</v>
       </c>
       <c r="W105" s="1" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.25">
@@ -7977,7 +7977,7 @@
         <v>158</v>
       </c>
       <c r="J106" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="K106" t="s">
         <v>159</v>
@@ -8007,7 +8007,7 @@
         <v>54</v>
       </c>
       <c r="W106" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="107" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -8030,7 +8030,7 @@
         <v>33</v>
       </c>
       <c r="J107" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="T107" t="s">
         <v>37</v>
@@ -8042,7 +8042,7 @@
         <v>54</v>
       </c>
       <c r="W107" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="108" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -8068,7 +8068,7 @@
         <v>168</v>
       </c>
       <c r="J108" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K108" t="s">
         <v>169</v>
@@ -8098,7 +8098,7 @@
         <v>54</v>
       </c>
       <c r="W108" s="1" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
     </row>
     <row r="109" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -8124,7 +8124,7 @@
         <v>168</v>
       </c>
       <c r="J109" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="K109" t="s">
         <v>175</v>
@@ -8154,7 +8154,7 @@
         <v>54</v>
       </c>
       <c r="W109" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.25">
@@ -8373,7 +8373,7 @@
         <v>195</v>
       </c>
       <c r="J115" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="K115" t="s">
         <v>194</v>
@@ -8420,7 +8420,7 @@
         <v>195</v>
       </c>
       <c r="J116" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="K116" t="s">
         <v>199</v>
@@ -8467,7 +8467,7 @@
         <v>195</v>
       </c>
       <c r="J117" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="K117" t="s">
         <v>203</v>
@@ -8514,7 +8514,7 @@
         <v>195</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K118" s="1" t="s">
         <v>208</v>
@@ -8529,7 +8529,7 @@
         <v>54</v>
       </c>
       <c r="W118" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
@@ -8555,7 +8555,7 @@
         <v>195</v>
       </c>
       <c r="J119" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="K119" t="s">
         <v>210</v>
@@ -8602,7 +8602,7 @@
         <v>215</v>
       </c>
       <c r="J120" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="K120" t="s">
         <v>214</v>
@@ -8763,7 +8763,7 @@
         <v>225</v>
       </c>
       <c r="J124" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="K124" t="s">
         <v>232</v>
@@ -8854,7 +8854,7 @@
         <v>243</v>
       </c>
       <c r="J126" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="K126" t="s">
         <v>241</v>
@@ -8942,7 +8942,7 @@
         <v>252</v>
       </c>
       <c r="J128" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="K128" t="s">
         <v>253</v>
@@ -9092,7 +9092,7 @@
         <v>266</v>
       </c>
       <c r="J131" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="K131" t="s">
         <v>267</v>
@@ -9148,7 +9148,7 @@
         <v>275</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="K132" t="s">
         <v>276</v>
@@ -9178,7 +9178,7 @@
         <v>281</v>
       </c>
       <c r="W132" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="133" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -9204,7 +9204,7 @@
         <v>275</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K133" s="1" t="s">
         <v>285</v>
@@ -9237,7 +9237,7 @@
         <v>281</v>
       </c>
       <c r="W133" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="134" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -9263,7 +9263,7 @@
         <v>275</v>
       </c>
       <c r="J134" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K134" t="s">
         <v>293</v>
@@ -9322,7 +9322,7 @@
         <v>301</v>
       </c>
       <c r="J135" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K135" t="s">
         <v>293</v>
@@ -9381,7 +9381,7 @@
         <v>275</v>
       </c>
       <c r="J136" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="K136" t="s">
         <v>305</v>
@@ -9437,7 +9437,7 @@
         <v>275</v>
       </c>
       <c r="J137" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K137" t="s">
         <v>309</v>
@@ -9493,7 +9493,7 @@
         <v>275</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K138" t="s">
         <v>314</v>
@@ -9523,7 +9523,7 @@
         <v>281</v>
       </c>
       <c r="W138" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="X138" t="s">
         <v>318</v>
@@ -9552,7 +9552,7 @@
         <v>275</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K139" t="s">
         <v>314</v>
@@ -9582,7 +9582,7 @@
         <v>281</v>
       </c>
       <c r="W139" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="X139" t="s">
         <v>318</v>
@@ -9611,7 +9611,7 @@
         <v>275</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K140" t="s">
         <v>314</v>
@@ -9641,7 +9641,7 @@
         <v>281</v>
       </c>
       <c r="W140" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="X140" t="s">
         <v>318</v>
@@ -9670,7 +9670,7 @@
         <v>275</v>
       </c>
       <c r="J141" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K141" t="s">
         <v>326</v>
@@ -9898,7 +9898,7 @@
         <v>42</v>
       </c>
       <c r="J147" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="K147" t="s">
         <v>341</v>
@@ -9989,7 +9989,7 @@
         <v>349</v>
       </c>
       <c r="J149" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K149" t="s">
         <v>350</v>
@@ -10045,7 +10045,7 @@
         <v>355</v>
       </c>
       <c r="J150" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K150" t="s">
         <v>356</v>
@@ -10104,7 +10104,7 @@
         <v>365</v>
       </c>
       <c r="J151" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="K151" t="s">
         <v>356</v>
@@ -10160,7 +10160,7 @@
         <v>369</v>
       </c>
       <c r="J152" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K152" t="s">
         <v>370</v>
@@ -10216,7 +10216,7 @@
         <v>376</v>
       </c>
       <c r="J153" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K153" t="s">
         <v>377</v>
@@ -10351,7 +10351,7 @@
         <v>391</v>
       </c>
       <c r="J156" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="K156" t="s">
         <v>392</v>
@@ -10384,7 +10384,7 @@
         <v>54</v>
       </c>
       <c r="W156" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="157" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -10486,7 +10486,7 @@
         <v>355</v>
       </c>
       <c r="J159" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="K159" s="1" t="s">
         <v>405</v>
@@ -10516,7 +10516,7 @@
         <v>54</v>
       </c>
       <c r="W159" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="160" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
@@ -10542,7 +10542,7 @@
         <v>412</v>
       </c>
       <c r="J160" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>405</v>
@@ -10572,7 +10572,7 @@
         <v>281</v>
       </c>
       <c r="W160" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="161" spans="1:23" ht="75" x14ac:dyDescent="0.25">
@@ -10712,7 +10712,7 @@
         <v>275</v>
       </c>
       <c r="J164" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="K164" t="s">
         <v>426</v>
@@ -10768,7 +10768,7 @@
         <v>275</v>
       </c>
       <c r="J165" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="K165" t="s">
         <v>434</v>
@@ -10821,7 +10821,7 @@
         <v>98</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="T166" t="s">
         <v>37</v>
@@ -10833,7 +10833,7 @@
         <v>54</v>
       </c>
       <c r="W166" s="1" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
     <row r="167" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
@@ -10859,7 +10859,7 @@
         <v>444</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="T167" t="s">
         <v>37</v>
@@ -10871,7 +10871,7 @@
         <v>54</v>
       </c>
       <c r="W167" s="1" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
     </row>
     <row r="168" spans="1:23" x14ac:dyDescent="0.25">
@@ -10973,7 +10973,7 @@
         <v>49</v>
       </c>
       <c r="J170" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="K170" t="s">
         <v>50</v>
@@ -10994,7 +10994,7 @@
         <v>54</v>
       </c>
       <c r="W170" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="171" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -11067,7 +11067,7 @@
         <v>68</v>
       </c>
       <c r="J172" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="K172" t="s">
         <v>69</v>
@@ -11158,7 +11158,7 @@
         <v>42</v>
       </c>
       <c r="J174" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="K174" t="s">
         <v>84</v>
@@ -11214,7 +11214,7 @@
         <v>93</v>
       </c>
       <c r="J175" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="K175" t="s">
         <v>84</v>
@@ -11269,6 +11269,18 @@
       <c r="J176" t="s">
         <v>43</v>
       </c>
+      <c r="T176" t="s">
+        <v>79</v>
+      </c>
+      <c r="U176" t="s">
+        <v>80</v>
+      </c>
+      <c r="V176" t="s">
+        <v>79</v>
+      </c>
+      <c r="W176" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="177" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A177">
@@ -11328,7 +11340,7 @@
         <v>42</v>
       </c>
       <c r="J178" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="K178" t="s">
         <v>84</v>
@@ -11384,7 +11396,7 @@
         <v>109</v>
       </c>
       <c r="J179" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="K179" t="s">
         <v>110</v>
@@ -11440,7 +11452,7 @@
         <v>118</v>
       </c>
       <c r="J180" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="K180" t="s">
         <v>110</v>
@@ -11534,7 +11546,7 @@
         <v>125</v>
       </c>
       <c r="J182" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="K182" t="s">
         <v>126</v>
@@ -11593,7 +11605,7 @@
         <v>132</v>
       </c>
       <c r="J183" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="T183" t="s">
         <v>37</v>
@@ -11605,7 +11617,7 @@
         <v>54</v>
       </c>
       <c r="W183" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="184" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -11631,7 +11643,7 @@
         <v>135</v>
       </c>
       <c r="J184" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K184" t="s">
         <v>136</v>
@@ -11690,7 +11702,7 @@
         <v>132</v>
       </c>
       <c r="J185" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="T185" t="s">
         <v>37</v>
@@ -11702,7 +11714,7 @@
         <v>54</v>
       </c>
       <c r="W185" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="186" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -11728,7 +11740,7 @@
         <v>143</v>
       </c>
       <c r="J186" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="K186" t="s">
         <v>144</v>
@@ -11787,7 +11799,7 @@
         <v>125</v>
       </c>
       <c r="J187" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="K187" t="s">
         <v>149</v>
@@ -11849,7 +11861,7 @@
         <v>132</v>
       </c>
       <c r="J188" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="K188" t="s">
         <v>149</v>
@@ -11882,7 +11894,7 @@
         <v>54</v>
       </c>
       <c r="W188" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="189" spans="1:24" x14ac:dyDescent="0.25">
@@ -11984,7 +11996,7 @@
         <v>168</v>
       </c>
       <c r="J191" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="K191" t="s">
         <v>169</v>
@@ -12014,7 +12026,7 @@
         <v>54</v>
       </c>
       <c r="W191" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="192" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -12040,7 +12052,7 @@
         <v>168</v>
       </c>
       <c r="J192" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="K192" t="s">
         <v>175</v>
@@ -12070,7 +12082,7 @@
         <v>54</v>
       </c>
       <c r="W192" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="193" spans="1:24" x14ac:dyDescent="0.25">
@@ -12289,7 +12301,7 @@
         <v>195</v>
       </c>
       <c r="J198" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="K198" t="s">
         <v>194</v>
@@ -12336,7 +12348,7 @@
         <v>195</v>
       </c>
       <c r="J199" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="K199" t="s">
         <v>199</v>
@@ -12383,7 +12395,7 @@
         <v>195</v>
       </c>
       <c r="J200" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K200" t="s">
         <v>203</v>
@@ -12430,7 +12442,7 @@
         <v>195</v>
       </c>
       <c r="J201" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="K201" s="1" t="s">
         <v>208</v>
@@ -12445,7 +12457,7 @@
         <v>54</v>
       </c>
       <c r="W201" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="202" spans="1:24" x14ac:dyDescent="0.25">
@@ -12471,7 +12483,7 @@
         <v>195</v>
       </c>
       <c r="J202" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="K202" t="s">
         <v>210</v>
@@ -12518,7 +12530,7 @@
         <v>215</v>
       </c>
       <c r="J203" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="K203" t="s">
         <v>214</v>
@@ -12679,7 +12691,7 @@
         <v>225</v>
       </c>
       <c r="J207" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K207" t="s">
         <v>232</v>
@@ -12770,7 +12782,7 @@
         <v>243</v>
       </c>
       <c r="J209" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="K209" t="s">
         <v>241</v>
@@ -12858,7 +12870,7 @@
         <v>252</v>
       </c>
       <c r="J211" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="K211" t="s">
         <v>253</v>
@@ -13008,7 +13020,7 @@
         <v>266</v>
       </c>
       <c r="J214" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K214" t="s">
         <v>267</v>
@@ -13064,7 +13076,7 @@
         <v>275</v>
       </c>
       <c r="J215" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K215" t="s">
         <v>276</v>
@@ -13094,7 +13106,7 @@
         <v>281</v>
       </c>
       <c r="W215" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="216" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -13120,7 +13132,7 @@
         <v>275</v>
       </c>
       <c r="J216" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="K216" s="1" t="s">
         <v>285</v>
@@ -13153,7 +13165,7 @@
         <v>281</v>
       </c>
       <c r="W216" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="217" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -13179,7 +13191,7 @@
         <v>275</v>
       </c>
       <c r="J217" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K217" t="s">
         <v>293</v>
@@ -13238,7 +13250,7 @@
         <v>301</v>
       </c>
       <c r="J218" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K218" t="s">
         <v>293</v>
@@ -13297,7 +13309,7 @@
         <v>275</v>
       </c>
       <c r="J219" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="K219" t="s">
         <v>305</v>
@@ -13353,7 +13365,7 @@
         <v>275</v>
       </c>
       <c r="J220" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K220" t="s">
         <v>309</v>
@@ -13409,7 +13421,7 @@
         <v>275</v>
       </c>
       <c r="J221" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K221" t="s">
         <v>314</v>
@@ -13439,7 +13451,7 @@
         <v>281</v>
       </c>
       <c r="W221" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="X221" t="s">
         <v>318</v>
@@ -13468,7 +13480,7 @@
         <v>275</v>
       </c>
       <c r="J222" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K222" t="s">
         <v>314</v>
@@ -13498,7 +13510,7 @@
         <v>281</v>
       </c>
       <c r="W222" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="X222" t="s">
         <v>318</v>
@@ -13527,7 +13539,7 @@
         <v>275</v>
       </c>
       <c r="J223" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K223" t="s">
         <v>314</v>
@@ -13557,7 +13569,7 @@
         <v>281</v>
       </c>
       <c r="W223" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="X223" t="s">
         <v>318</v>
@@ -13586,7 +13598,7 @@
         <v>275</v>
       </c>
       <c r="J224" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="K224" t="s">
         <v>326</v>
@@ -13814,7 +13826,7 @@
         <v>42</v>
       </c>
       <c r="J230" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="K230" t="s">
         <v>341</v>
@@ -13905,7 +13917,7 @@
         <v>349</v>
       </c>
       <c r="J232" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="K232" t="s">
         <v>350</v>
@@ -13961,7 +13973,7 @@
         <v>355</v>
       </c>
       <c r="J233" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="K233" t="s">
         <v>356</v>
@@ -14020,7 +14032,7 @@
         <v>365</v>
       </c>
       <c r="J234" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="K234" t="s">
         <v>356</v>
@@ -14076,7 +14088,7 @@
         <v>369</v>
       </c>
       <c r="J235" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K235" t="s">
         <v>370</v>
@@ -14132,7 +14144,7 @@
         <v>376</v>
       </c>
       <c r="J236" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="K236" t="s">
         <v>377</v>
@@ -14267,7 +14279,7 @@
         <v>391</v>
       </c>
       <c r="J239" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="K239" t="s">
         <v>392</v>
@@ -14300,7 +14312,7 @@
         <v>54</v>
       </c>
       <c r="W239" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="240" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -14402,7 +14414,7 @@
         <v>355</v>
       </c>
       <c r="J242" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="K242" s="1" t="s">
         <v>405</v>
@@ -14435,7 +14447,7 @@
         <v>54</v>
       </c>
       <c r="W242" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="243" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -14461,7 +14473,7 @@
         <v>412</v>
       </c>
       <c r="J243" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="K243" s="1" t="s">
         <v>405</v>
@@ -14494,7 +14506,7 @@
         <v>281</v>
       </c>
       <c r="W243" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="244" spans="1:24" ht="75" x14ac:dyDescent="0.25">
@@ -14634,7 +14646,7 @@
         <v>275</v>
       </c>
       <c r="J247" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="K247" t="s">
         <v>426</v>
@@ -14690,7 +14702,7 @@
         <v>275</v>
       </c>
       <c r="J248" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K248" t="s">
         <v>434</v>
@@ -14746,7 +14758,7 @@
         <v>98</v>
       </c>
       <c r="J249" s="1" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="T249" t="s">
         <v>37</v>
@@ -14758,7 +14770,7 @@
         <v>54</v>
       </c>
       <c r="W249" s="1" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
     </row>
     <row r="250" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -14784,7 +14796,7 @@
         <v>444</v>
       </c>
       <c r="J250" s="1" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="T250" t="s">
         <v>37</v>
@@ -14796,7 +14808,7 @@
         <v>54</v>
       </c>
       <c r="W250" s="1" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="254" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>